<commit_message>
Obtain grid search results
</commit_message>
<xml_diff>
--- a/resultats/cnn_gridsearch.xlsx
+++ b/resultats/cnn_gridsearch.xlsx
@@ -9,14 +9,15 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="860" yWindow="440" windowWidth="27940" windowHeight="17560" tabRatio="500"/>
+    <workbookView xWindow="860" yWindow="440" windowWidth="25760" windowHeight="17560" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="Essai" sheetId="1" r:id="rId1"/>
+    <sheet name="MNIST-CNN1" sheetId="2" r:id="rId1"/>
+    <sheet name="Essai" sheetId="1" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="gridsearch" localSheetId="0">Essai!$C$6:$G$10</definedName>
-    <definedName name="gridsearch_1" localSheetId="0">Essai!$J$4:$N$8</definedName>
+    <definedName name="gridsearch" localSheetId="1">Essai!$C$6:$G$10</definedName>
+    <definedName name="gridsearch_1" localSheetId="0">'MNIST-CNN1'!$C$5:$G$9</definedName>
   </definedNames>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -33,7 +34,7 @@
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <connection id="1" name="gridsearch" type="6" refreshedVersion="0" background="1" saveData="1">
-    <textPr fileType="mac" codePage="10000" sourceFile="/Users/carl/Documents/uni/RecFormesAnalyseIm/Analyse_dimage_avance_proj/gridsearch.csv" thousands=" ">
+    <textPr fileType="mac" sourceFile="/Users/carl/Documents/uni/RecFormesAnalyseIm/Analyse_dimage_avance_proj/gridsearch.csv" thousands=" ">
       <textFields count="5">
         <textField/>
         <textField/>
@@ -44,7 +45,7 @@
     </textPr>
   </connection>
   <connection id="2" name="gridsearch1" type="6" refreshedVersion="0" background="1" saveData="1">
-    <textPr fileType="mac" codePage="10000" sourceFile="/Users/carl/Documents/uni/RecFormesAnalyseIm/Analyse_dimage_avance_proj/gridsearch.csv" thousands=" ">
+    <textPr fileType="mac" sourceFile="/Users/carl/Documents/uni/RecFormesAnalyseIm/Analyse_dimage_avance_proj/gridsearch.csv" thousands=" ">
       <textFields count="5">
         <textField/>
         <textField/>
@@ -58,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="3">
   <si>
     <t>Batch size</t>
   </si>
@@ -73,7 +74,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -96,13 +97,31 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC00000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -132,17 +151,22 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="10" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -428,239 +452,241 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:N10"/>
+  <dimension ref="A3:I12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="L27" sqref="L27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="6.6640625" customWidth="1"/>
-    <col min="2" max="2" width="4.33203125" customWidth="1"/>
-    <col min="3" max="6" width="9.6640625" customWidth="1"/>
-    <col min="10" max="14" width="8.1640625" customWidth="1"/>
+    <col min="2" max="2" width="5.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="C2" s="5" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="C4" s="2" t="s">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="C3" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-      <c r="J4" s="1">
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4"/>
+      <c r="I3" s="4"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="C4" s="2">
+        <v>64</v>
+      </c>
+      <c r="D4" s="2">
+        <v>128</v>
+      </c>
+      <c r="E4" s="2">
+        <v>256</v>
+      </c>
+      <c r="F4" s="2">
+        <v>512</v>
+      </c>
+      <c r="G4" s="2">
+        <v>1024</v>
+      </c>
+      <c r="H4" s="7">
+        <v>2048</v>
+      </c>
+      <c r="I4" s="7">
+        <v>4096</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" s="2">
+        <v>4</v>
+      </c>
+      <c r="C5" s="1">
         <v>0.95799999999999896</v>
       </c>
-      <c r="K4" s="1">
+      <c r="D5" s="1">
         <v>0.96550000000000002</v>
       </c>
-      <c r="L4" s="1">
+      <c r="E5" s="1">
         <v>0.96709999999999896</v>
       </c>
-      <c r="M4" s="1">
+      <c r="F5" s="1">
         <v>0.96889999999999898</v>
       </c>
-      <c r="N4" s="1">
+      <c r="G5" s="1">
         <v>0.96960000000000002</v>
       </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="C5" s="3">
+      <c r="H5" s="1">
+        <v>0.90900000000000003</v>
+      </c>
+      <c r="I5" s="1">
+        <v>0.94200000000000006</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6" s="5"/>
+      <c r="B6" s="2">
+        <v>8</v>
+      </c>
+      <c r="C6" s="1">
+        <v>0.974799999999999</v>
+      </c>
+      <c r="D6" s="1">
+        <v>0.98089999999999899</v>
+      </c>
+      <c r="E6" s="1">
+        <v>0.98270000000000002</v>
+      </c>
+      <c r="F6" s="1">
+        <v>0.98529999999999895</v>
+      </c>
+      <c r="G6" s="1">
+        <v>0.98670000000000002</v>
+      </c>
+      <c r="H6" s="1">
+        <v>0.94399999999999995</v>
+      </c>
+      <c r="I6" s="1">
+        <v>0.95299999999999996</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A7" s="5"/>
+      <c r="B7" s="2">
+        <v>16</v>
+      </c>
+      <c r="C7" s="1">
+        <v>0.98240000000000005</v>
+      </c>
+      <c r="D7" s="1">
+        <v>0.98799999999999899</v>
+      </c>
+      <c r="E7" s="1">
+        <v>0.99060000000000004</v>
+      </c>
+      <c r="F7" s="1">
+        <v>0.9909</v>
+      </c>
+      <c r="G7" s="1">
+        <v>0.99050000000000005</v>
+      </c>
+      <c r="H7" s="1">
+        <v>0.95199999999999996</v>
+      </c>
+      <c r="I7" s="1">
+        <v>0.96400000000000008</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A8" s="5"/>
+      <c r="B8" s="2">
+        <v>32</v>
+      </c>
+      <c r="C8" s="1">
+        <v>0.98970000000000002</v>
+      </c>
+      <c r="D8" s="1">
+        <v>0.99229999999999896</v>
+      </c>
+      <c r="E8" s="1">
+        <v>0.99250000000000005</v>
+      </c>
+      <c r="F8" s="1">
+        <v>0.99390000000000001</v>
+      </c>
+      <c r="G8" s="1">
+        <v>0.99409999999999898</v>
+      </c>
+      <c r="H8" s="1">
+        <v>0.95399999999999996</v>
+      </c>
+      <c r="I8" s="1">
+        <v>0.96900000000000008</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A9" s="5"/>
+      <c r="B9" s="2">
         <v>64</v>
       </c>
-      <c r="D5" s="3">
+      <c r="C9" s="1">
+        <v>0.99029999999999896</v>
+      </c>
+      <c r="D9" s="1">
+        <v>0.99339999999999895</v>
+      </c>
+      <c r="E9" s="1">
+        <v>0.99409999999999898</v>
+      </c>
+      <c r="F9" s="1">
+        <v>0.99450000000000005</v>
+      </c>
+      <c r="G9" s="1">
+        <v>0.99409999999999898</v>
+      </c>
+      <c r="H9" s="1">
+        <v>0.96799999999999997</v>
+      </c>
+      <c r="I9" s="6">
+        <v>0.97799999999999998</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A10" s="5"/>
+      <c r="B10" s="7">
         <v>128</v>
       </c>
-      <c r="E5" s="3">
+      <c r="C10" s="1">
+        <v>0.99199999999999999</v>
+      </c>
+      <c r="D10" s="1">
+        <v>0.99400000000000011</v>
+      </c>
+      <c r="E10" s="1">
+        <v>0.99400000000000011</v>
+      </c>
+      <c r="F10" s="1">
+        <v>0.995</v>
+      </c>
+      <c r="G10" s="1">
+        <v>0.995</v>
+      </c>
+      <c r="H10" s="1">
+        <v>0.995</v>
+      </c>
+      <c r="I10" s="1">
+        <v>0.995</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A11" s="5"/>
+      <c r="B11" s="7">
         <v>256</v>
       </c>
-      <c r="F5" s="3">
-        <v>512</v>
-      </c>
-      <c r="G5" s="3">
-        <v>1024</v>
-      </c>
-      <c r="J5" s="1">
-        <v>0.974799999999999</v>
-      </c>
-      <c r="K5" s="1">
-        <v>0.98089999999999899</v>
-      </c>
-      <c r="L5" s="1">
-        <v>0.98270000000000002</v>
-      </c>
-      <c r="M5" s="1">
-        <v>0.98529999999999895</v>
-      </c>
-      <c r="N5" s="1">
-        <v>0.98670000000000002</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A6" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B6" s="3">
-        <v>4</v>
-      </c>
-      <c r="C6" s="1">
-        <v>0.96619999999999895</v>
-      </c>
-      <c r="D6" s="1">
-        <v>0.97440000000000004</v>
-      </c>
-      <c r="E6" s="1">
-        <v>0.97899999999999898</v>
-      </c>
-      <c r="F6" s="1">
-        <v>0.97960000000000003</v>
-      </c>
-      <c r="G6" s="1">
-        <v>0.98109999999999897</v>
-      </c>
-      <c r="J6" s="1">
-        <v>0.98240000000000005</v>
-      </c>
-      <c r="K6" s="1">
-        <v>0.98799999999999899</v>
-      </c>
-      <c r="L6" s="1">
-        <v>0.99060000000000004</v>
-      </c>
-      <c r="M6" s="1">
-        <v>0.9909</v>
-      </c>
-      <c r="N6" s="1">
-        <v>0.99050000000000005</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A7" s="4"/>
-      <c r="B7" s="3">
-        <v>8</v>
-      </c>
-      <c r="C7" s="1">
-        <v>0.97989999999999899</v>
-      </c>
-      <c r="D7" s="1">
-        <v>0.98570000000000002</v>
-      </c>
-      <c r="E7" s="1">
-        <v>0.98660000000000003</v>
-      </c>
-      <c r="F7" s="1">
-        <v>0.98760000000000003</v>
-      </c>
-      <c r="G7" s="1">
-        <v>0.98870000000000002</v>
-      </c>
-      <c r="J7" s="1">
-        <v>0.98970000000000002</v>
-      </c>
-      <c r="K7" s="1">
-        <v>0.99229999999999896</v>
-      </c>
-      <c r="L7" s="1">
-        <v>0.99250000000000005</v>
-      </c>
-      <c r="M7" s="1">
-        <v>0.99390000000000001</v>
-      </c>
-      <c r="N7" s="1">
-        <v>0.99409999999999898</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A8" s="4"/>
-      <c r="B8" s="3">
-        <v>16</v>
-      </c>
-      <c r="C8" s="1">
-        <v>0.98440000000000005</v>
-      </c>
-      <c r="D8" s="1">
-        <v>0.98709999999999898</v>
-      </c>
-      <c r="E8" s="1">
-        <v>0.98960000000000004</v>
-      </c>
-      <c r="F8" s="1">
-        <v>0.98960000000000004</v>
-      </c>
-      <c r="G8" s="1">
-        <v>0.9899</v>
-      </c>
-      <c r="J8" s="1">
-        <v>0.99029999999999896</v>
-      </c>
-      <c r="K8" s="1">
-        <v>0.99339999999999895</v>
-      </c>
-      <c r="L8" s="1">
-        <v>0.99409999999999898</v>
-      </c>
-      <c r="M8" s="1">
-        <v>0.99450000000000005</v>
-      </c>
-      <c r="N8" s="1">
-        <v>0.99409999999999898</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A9" s="4"/>
-      <c r="B9" s="3">
-        <v>32</v>
-      </c>
-      <c r="C9" s="1">
-        <v>0.98860000000000003</v>
-      </c>
-      <c r="D9" s="1">
-        <v>0.99039999999999895</v>
-      </c>
-      <c r="E9" s="1">
-        <v>0.99080000000000001</v>
-      </c>
-      <c r="F9" s="1">
-        <v>0.99119999999999897</v>
-      </c>
-      <c r="G9" s="1">
-        <v>0.99129999999999896</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A10" s="4"/>
-      <c r="B10" s="3">
-        <v>64</v>
-      </c>
-      <c r="C10" s="1">
-        <v>0.98799999999999899</v>
-      </c>
-      <c r="D10" s="1">
-        <v>0.99060000000000004</v>
-      </c>
-      <c r="E10" s="1">
-        <v>0.99180000000000001</v>
-      </c>
-      <c r="F10" s="1">
-        <v>0.99160000000000004</v>
-      </c>
-      <c r="G10" s="1">
-        <v>0.99180000000000001</v>
-      </c>
+      <c r="C11" s="10">
+        <v>0.114</v>
+      </c>
+      <c r="D11" s="10">
+        <v>0.114</v>
+      </c>
+      <c r="E11" s="9"/>
+      <c r="F11" s="9"/>
+      <c r="G11" s="9"/>
+      <c r="H11" s="9"/>
+      <c r="I11" s="9"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B12" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="C4:G4"/>
-    <mergeCell ref="A6:A10"/>
+    <mergeCell ref="C3:I3"/>
+    <mergeCell ref="A5:A11"/>
   </mergeCells>
-  <conditionalFormatting sqref="C6:G10">
+  <conditionalFormatting sqref="C5:G9 C11:I11">
     <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="min"/>
@@ -672,7 +698,19 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J4:N8">
+  <conditionalFormatting sqref="C7:G9 C11:I11">
+    <cfRule type="colorScale" priority="4">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C5:I12">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
@@ -684,7 +722,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J6:N8">
+  <conditionalFormatting sqref="C5:I10">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
@@ -698,4 +736,179 @@
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:G10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E35" sqref="E35"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="6.6640625" customWidth="1"/>
+    <col min="2" max="2" width="4.33203125" customWidth="1"/>
+    <col min="3" max="6" width="9.6640625" customWidth="1"/>
+    <col min="10" max="14" width="8.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C2" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C4" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C5" s="2">
+        <v>64</v>
+      </c>
+      <c r="D5" s="2">
+        <v>128</v>
+      </c>
+      <c r="E5" s="2">
+        <v>256</v>
+      </c>
+      <c r="F5" s="2">
+        <v>512</v>
+      </c>
+      <c r="G5" s="2">
+        <v>1024</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6" s="2">
+        <v>4</v>
+      </c>
+      <c r="C6" s="1">
+        <v>0.96619999999999895</v>
+      </c>
+      <c r="D6" s="1">
+        <v>0.97440000000000004</v>
+      </c>
+      <c r="E6" s="1">
+        <v>0.97899999999999898</v>
+      </c>
+      <c r="F6" s="1">
+        <v>0.97960000000000003</v>
+      </c>
+      <c r="G6" s="1">
+        <v>0.98109999999999897</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" s="5"/>
+      <c r="B7" s="2">
+        <v>8</v>
+      </c>
+      <c r="C7" s="1">
+        <v>0.97989999999999899</v>
+      </c>
+      <c r="D7" s="1">
+        <v>0.98570000000000002</v>
+      </c>
+      <c r="E7" s="1">
+        <v>0.98660000000000003</v>
+      </c>
+      <c r="F7" s="1">
+        <v>0.98760000000000003</v>
+      </c>
+      <c r="G7" s="1">
+        <v>0.98870000000000002</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" s="5"/>
+      <c r="B8" s="2">
+        <v>16</v>
+      </c>
+      <c r="C8" s="1">
+        <v>0.98440000000000005</v>
+      </c>
+      <c r="D8" s="1">
+        <v>0.98709999999999898</v>
+      </c>
+      <c r="E8" s="1">
+        <v>0.98960000000000004</v>
+      </c>
+      <c r="F8" s="1">
+        <v>0.98960000000000004</v>
+      </c>
+      <c r="G8" s="1">
+        <v>0.9899</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" s="5"/>
+      <c r="B9" s="2">
+        <v>32</v>
+      </c>
+      <c r="C9" s="1">
+        <v>0.98860000000000003</v>
+      </c>
+      <c r="D9" s="1">
+        <v>0.99039999999999895</v>
+      </c>
+      <c r="E9" s="1">
+        <v>0.99080000000000001</v>
+      </c>
+      <c r="F9" s="1">
+        <v>0.99119999999999897</v>
+      </c>
+      <c r="G9" s="1">
+        <v>0.99129999999999896</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" s="5"/>
+      <c r="B10" s="2">
+        <v>64</v>
+      </c>
+      <c r="C10" s="1">
+        <v>0.98799999999999899</v>
+      </c>
+      <c r="D10" s="1">
+        <v>0.99060000000000004</v>
+      </c>
+      <c r="E10" s="1">
+        <v>0.99180000000000001</v>
+      </c>
+      <c r="F10" s="1">
+        <v>0.99160000000000004</v>
+      </c>
+      <c r="G10" s="1">
+        <v>0.99180000000000001</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="C4:G4"/>
+    <mergeCell ref="A6:A10"/>
+  </mergeCells>
+  <conditionalFormatting sqref="C6:G10">
+    <cfRule type="colorScale" priority="4">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Prevent retention of weights; Redo cifar10
</commit_message>
<xml_diff>
--- a/resultats/cnn_gridsearch.xlsx
+++ b/resultats/cnn_gridsearch.xlsx
@@ -17,9 +17,10 @@
     <sheet name="Essai" sheetId="1" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="gridsearch" localSheetId="1">'CIFAR10-CNN1'!$C$5:$F$7</definedName>
     <definedName name="gridsearch" localSheetId="2">Essai!$C$6:$G$10</definedName>
+    <definedName name="gridsearch_1" localSheetId="1">'CIFAR10-CNN1'!$C$19:$I$25</definedName>
     <definedName name="gridsearch_1" localSheetId="0">'MNIST-CNN1'!$C$5:$G$9</definedName>
+    <definedName name="gridsearch_2" localSheetId="1">'CIFAR10-CNN1'!$C$5:$G$10</definedName>
   </definedNames>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -57,9 +58,23 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="3" name="gridsearch2" type="6" refreshedVersion="0" background="1" saveData="1">
+  <connection id="3" name="gridsearch3" type="6" refreshedVersion="0" background="1" saveData="1">
+    <textPr fileType="mac" sourceFile="/Users/carl/Documents/uni/RecFormesAnalyseIm/Analyse_dimage_avance_proj/gridsearch.csv" thousands=" ">
+      <textFields count="7">
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="4" name="gridsearch4" type="6" refreshedVersion="0" background="1" saveData="1">
     <textPr fileType="mac" codePage="10000" sourceFile="/Users/carl/Documents/uni/RecFormesAnalyseIm/Analyse_dimage_avance_proj/gridsearch.csv" thousands=" ">
-      <textFields count="4">
+      <textFields count="5">
+        <textField/>
         <textField/>
         <textField/>
         <textField/>
@@ -71,7 +86,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="65">
   <si>
     <t>Batch size</t>
   </si>
@@ -85,17 +100,345 @@
     <t>Nb. epochs: 6   Kernel size: (3, 3)   Pool size: (2, 2)</t>
   </si>
   <si>
-    <t>First filter size*</t>
-  </si>
-  <si>
-    <t>* Tailles de filtre pour les 4 couches : [n, 2n, 4n, 8n]</t>
+    <t>Layer (type)</t>
+  </si>
+  <si>
+    <t>Output Shape</t>
+  </si>
+  <si>
+    <t>Param #</t>
+  </si>
+  <si>
+    <t>Connected to</t>
+  </si>
+  <si>
+    <t>convolution2d_1 (Convolution2D)</t>
+  </si>
+  <si>
+    <t>convolution2d_input_1[0][0]</t>
+  </si>
+  <si>
+    <t>activation_1 (Activation)</t>
+  </si>
+  <si>
+    <t>convolution2d_1[0][0]</t>
+  </si>
+  <si>
+    <t>convolution2d_2 (Convolution2D)</t>
+  </si>
+  <si>
+    <t>activation_1[0][0]</t>
+  </si>
+  <si>
+    <t>activation_2 (Activation)</t>
+  </si>
+  <si>
+    <t>convolution2d_2[0][0]</t>
+  </si>
+  <si>
+    <t>maxpooling2d_1 (MaxPooling2D)</t>
+  </si>
+  <si>
+    <t>activation_2[0][0]</t>
+  </si>
+  <si>
+    <t>dropout_1 (Dropout)</t>
+  </si>
+  <si>
+    <t>maxpooling2d_1[0][0]</t>
+  </si>
+  <si>
+    <t>convolution2d_3 (Convolution2D)</t>
+  </si>
+  <si>
+    <t>dropout_1[0][0]</t>
+  </si>
+  <si>
+    <t>activation_3 (Activation)</t>
+  </si>
+  <si>
+    <t>convolution2d_3[0][0]</t>
+  </si>
+  <si>
+    <t>convolution2d_4 (Convolution2D)</t>
+  </si>
+  <si>
+    <t>activation_3[0][0]</t>
+  </si>
+  <si>
+    <t>activation_4 (Activation)</t>
+  </si>
+  <si>
+    <t>convolution2d_4[0][0]</t>
+  </si>
+  <si>
+    <t>maxpooling2d_2 (MaxPooling2D)</t>
+  </si>
+  <si>
+    <t>activation_4[0][0]</t>
+  </si>
+  <si>
+    <t>dropout_2 (Dropout)</t>
+  </si>
+  <si>
+    <t>maxpooling2d_2[0][0]</t>
+  </si>
+  <si>
+    <t>flatten_1 (Flatten)</t>
+  </si>
+  <si>
+    <t>(None, 3200)</t>
+  </si>
+  <si>
+    <t>dropout_2[0][0]</t>
+  </si>
+  <si>
+    <t>dense_1 (Dense)</t>
+  </si>
+  <si>
+    <t>(None, 128)</t>
+  </si>
+  <si>
+    <t>flatten_1[0][0]</t>
+  </si>
+  <si>
+    <t>activation_5 (Activation)</t>
+  </si>
+  <si>
+    <t>dense_1[0][0]</t>
+  </si>
+  <si>
+    <t>dropout_3 (Dropout)</t>
+  </si>
+  <si>
+    <t>activation_5[0][0]</t>
+  </si>
+  <si>
+    <t>dense_2 (Dense)</t>
+  </si>
+  <si>
+    <t>(None, 10)</t>
+  </si>
+  <si>
+    <t>dropout_3[0][0]</t>
+  </si>
+  <si>
+    <t>activation_6 (Activation)</t>
+  </si>
+  <si>
+    <t>dense_2[0][0]</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">(None, 30, 30, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>16</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">(None, 28, 28, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>32</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">(None, 14, 14, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>32</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">(None, 12, 12, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>64</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">(None, 10, 10, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>128</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">(None, 5, 5, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>128)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">(None, 5, 5, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>128</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <t>Exemple de configuration. Le nombre de filtres dans chaque couche varie dans le grid search.</t>
+  </si>
+  <si>
+    <t>Total params:</t>
+  </si>
+  <si>
+    <t>4, 8, 16, 32</t>
+  </si>
+  <si>
+    <t>8, 8, 16, 16</t>
+  </si>
+  <si>
+    <t>8, 16, 32, 64</t>
+  </si>
+  <si>
+    <t>16, 16, 32, 32</t>
+  </si>
+  <si>
+    <t>16, 32, 64, 128</t>
+  </si>
+  <si>
+    <t>32, 32, 64, 64</t>
+  </si>
+  <si>
+    <t>Nb. epochs: 10   Kernel size: (3, 3)   Pool size: (2, 2)</t>
+  </si>
+  <si>
+    <t>Filter config</t>
+  </si>
+  <si>
+    <t>Refaire car persistence des poids</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -125,14 +468,35 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10"/>
+      <sz val="12"/>
       <color theme="1"/>
+      <name val="Andale Mono"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -151,8 +515,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -175,11 +545,70 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -189,17 +618,82 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="10" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="10" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="10" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="51">
+    <cellStyle name="Lien hypertexte" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="50" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -217,10 +711,14 @@
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="gridsearch" connectionId="3" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="gridsearch_2" connectionId="4" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="gridsearch_1" connectionId="3" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="gridsearch" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
@@ -487,10 +985,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I12"/>
+  <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G27" sqref="G27"/>
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -504,15 +1002,15 @@
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="C3" s="9" t="s">
+      <c r="C3" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="9"/>
-      <c r="E3" s="9"/>
-      <c r="F3" s="9"/>
-      <c r="G3" s="9"/>
-      <c r="H3" s="9"/>
-      <c r="I3" s="9"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="19"/>
+      <c r="F3" s="19"/>
+      <c r="G3" s="19"/>
+      <c r="H3" s="19"/>
+      <c r="I3" s="19"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C4" s="2">
@@ -538,7 +1036,7 @@
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A5" s="10" t="s">
+      <c r="A5" s="20" t="s">
         <v>1</v>
       </c>
       <c r="B5" s="2">
@@ -567,7 +1065,7 @@
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A6" s="10"/>
+      <c r="A6" s="20"/>
       <c r="B6" s="2">
         <v>8</v>
       </c>
@@ -594,7 +1092,7 @@
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A7" s="10"/>
+      <c r="A7" s="20"/>
       <c r="B7" s="2">
         <v>16</v>
       </c>
@@ -621,7 +1119,7 @@
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A8" s="10"/>
+      <c r="A8" s="20"/>
       <c r="B8" s="2">
         <v>32</v>
       </c>
@@ -648,7 +1146,7 @@
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A9" s="10"/>
+      <c r="A9" s="20"/>
       <c r="B9" s="2">
         <v>64</v>
       </c>
@@ -675,7 +1173,7 @@
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A10" s="10"/>
+      <c r="A10" s="20"/>
       <c r="B10" s="5">
         <v>128</v>
       </c>
@@ -702,7 +1200,7 @@
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A11" s="10"/>
+      <c r="A11" s="20"/>
       <c r="B11" s="5">
         <v>256</v>
       </c>
@@ -720,6 +1218,17 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B12" s="6"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A13" s="22" t="s">
+        <v>64</v>
+      </c>
+      <c r="B13" s="22"/>
+      <c r="C13" s="22"/>
+      <c r="D13" s="22"/>
+      <c r="E13" s="22"/>
+      <c r="F13" s="22"/>
+      <c r="G13" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -780,182 +1289,800 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I12"/>
+  <dimension ref="A1:S53"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G19" sqref="G19"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="6" width="8.1640625" customWidth="1"/>
+    <col min="1" max="1" width="7.6640625" customWidth="1"/>
+    <col min="2" max="2" width="13.33203125" customWidth="1"/>
+    <col min="3" max="9" width="8.1640625" customWidth="1"/>
+    <col min="12" max="12" width="30.6640625" customWidth="1"/>
+    <col min="13" max="13" width="18.1640625" customWidth="1"/>
+    <col min="14" max="14" width="9" customWidth="1"/>
+    <col min="15" max="15" width="25.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="C3" s="9" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L2" s="16" t="s">
+        <v>54</v>
+      </c>
+      <c r="M2" s="16"/>
+      <c r="N2" s="16"/>
+      <c r="O2" s="16"/>
+      <c r="P2" s="12"/>
+      <c r="Q2" s="12"/>
+      <c r="R2" s="12"/>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="C3" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="9"/>
-      <c r="E3" s="9"/>
-      <c r="F3" s="9"/>
-      <c r="G3" s="9"/>
-      <c r="H3" s="9"/>
-      <c r="I3" s="9"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="D3" s="19"/>
+      <c r="E3" s="19"/>
+      <c r="F3" s="19"/>
+      <c r="G3" s="19"/>
+      <c r="H3" s="21"/>
+      <c r="I3" s="21"/>
+      <c r="L3" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="M3" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="N3" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="O3" s="13" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
       <c r="C4" s="2">
+        <v>8</v>
+      </c>
+      <c r="D4" s="2">
+        <v>16</v>
+      </c>
+      <c r="E4" s="2">
+        <v>32</v>
+      </c>
+      <c r="F4" s="2">
         <v>64</v>
       </c>
-      <c r="D4" s="2">
+      <c r="G4" s="2">
         <v>128</v>
       </c>
-      <c r="E4" s="2">
-        <v>256</v>
-      </c>
-      <c r="F4" s="2">
-        <v>512</v>
-      </c>
-      <c r="G4" s="2">
-        <v>1024</v>
-      </c>
-      <c r="H4" s="5">
-        <v>2048</v>
-      </c>
-      <c r="I4" s="5">
-        <v>4096</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A5" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="2">
-        <v>4</v>
+      <c r="H4" s="6"/>
+      <c r="I4" s="6"/>
+      <c r="L4" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="M4" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="N4" s="12">
+        <v>448</v>
+      </c>
+      <c r="O4" s="12" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="20" t="s">
+        <v>63</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>56</v>
       </c>
       <c r="C5" s="1">
-        <v>0.48549999999999899</v>
+        <v>0.58009999999999895</v>
       </c>
       <c r="D5" s="1">
-        <v>0.5403</v>
+        <v>0.59189999999999898</v>
       </c>
       <c r="E5" s="1">
-        <v>0.56440000000000001</v>
+        <v>0.54879999999999896</v>
       </c>
       <c r="F5" s="1">
-        <v>0.58409999999999895</v>
-      </c>
-      <c r="G5" s="1"/>
+        <v>0.52480000000000004</v>
+      </c>
+      <c r="G5" s="1">
+        <v>0.502</v>
+      </c>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A6" s="10"/>
-      <c r="B6" s="2">
-        <v>8</v>
+      <c r="L5" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="M5" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="N5" s="14">
+        <v>0</v>
+      </c>
+      <c r="O5" s="14" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A6" s="20"/>
+      <c r="B6" s="2" t="s">
+        <v>57</v>
       </c>
       <c r="C6" s="1">
-        <v>0.55089999999999895</v>
+        <v>0.54020000000000001</v>
       </c>
       <c r="D6" s="1">
-        <v>0.60640000000000005</v>
+        <v>0.56259999999999899</v>
       </c>
       <c r="E6" s="1">
-        <v>0.63239999999999896</v>
+        <v>0.56499999999999895</v>
       </c>
       <c r="F6" s="1">
-        <v>0.66020000000000001</v>
-      </c>
-      <c r="G6" s="1"/>
+        <v>0.52710000000000001</v>
+      </c>
+      <c r="G6" s="1">
+        <v>0.50839999999999896</v>
+      </c>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A7" s="10"/>
-      <c r="B7" s="2">
-        <v>16</v>
+      <c r="L6" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="M6" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="N6" s="12">
+        <v>4640</v>
+      </c>
+      <c r="O6" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="S6" s="11"/>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A7" s="20"/>
+      <c r="B7" s="2" t="s">
+        <v>58</v>
       </c>
       <c r="C7" s="1">
-        <v>0.59150000000000003</v>
+        <v>0.65890000000000004</v>
       </c>
       <c r="D7" s="1">
-        <v>0.68230000000000002</v>
+        <v>0.65149999999999897</v>
       </c>
       <c r="E7" s="1">
-        <v>0.70930000000000004</v>
+        <v>0.63880000000000003</v>
       </c>
       <c r="F7" s="1">
-        <v>0.72889999999999899</v>
-      </c>
-      <c r="G7" s="1"/>
+        <v>0.61519999999999897</v>
+      </c>
+      <c r="G7" s="1">
+        <v>0.5776</v>
+      </c>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A8" s="10"/>
-      <c r="B8" s="2">
-        <v>32</v>
-      </c>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
-      <c r="G8" s="1"/>
+      <c r="L7" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="M7" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="N7" s="12">
+        <v>0</v>
+      </c>
+      <c r="O7" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="S7" s="11"/>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A8" s="20"/>
+      <c r="B8" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C8" s="1">
+        <v>0.63929999999999898</v>
+      </c>
+      <c r="D8" s="1">
+        <v>0.6391</v>
+      </c>
+      <c r="E8" s="1">
+        <v>0.60089999999999899</v>
+      </c>
+      <c r="F8" s="1">
+        <v>0.60289999999999899</v>
+      </c>
+      <c r="G8" s="1">
+        <v>0.56889999999999896</v>
+      </c>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A9" s="10"/>
-      <c r="B9" s="2">
-        <v>64</v>
-      </c>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
-      <c r="H9" s="1"/>
+      <c r="L8" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="M8" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="N8" s="12">
+        <v>0</v>
+      </c>
+      <c r="O8" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="S8" s="11"/>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A9" s="20"/>
+      <c r="B9" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C9" s="1">
+        <v>0.69599999999999895</v>
+      </c>
+      <c r="D9" s="1">
+        <v>0.681499999999999</v>
+      </c>
+      <c r="E9" s="1">
+        <v>0.67500000000000004</v>
+      </c>
+      <c r="F9" s="1">
+        <v>0.64490000000000003</v>
+      </c>
+      <c r="G9" s="1">
+        <v>0.61750000000000005</v>
+      </c>
+      <c r="H9" s="10"/>
       <c r="I9" s="4"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A10" s="10"/>
-      <c r="B10" s="5">
-        <v>128</v>
-      </c>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
+      <c r="L9" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="M9" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="N9" s="14">
+        <v>0</v>
+      </c>
+      <c r="O9" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="S9" s="11"/>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A10" s="20"/>
+      <c r="B10" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C10" s="1">
+        <v>0.70150000000000001</v>
+      </c>
+      <c r="D10" s="1">
+        <v>0.71360000000000001</v>
+      </c>
+      <c r="E10" s="1">
+        <v>0.64859999999999995</v>
+      </c>
+      <c r="F10" s="1">
+        <v>0.65239999999999998</v>
+      </c>
+      <c r="G10" s="1">
+        <v>0.61180000000000001</v>
+      </c>
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A11" s="10"/>
-      <c r="B11" s="5">
-        <v>256</v>
-      </c>
-      <c r="C11" s="11"/>
-      <c r="D11" s="11"/>
-      <c r="E11" s="12"/>
-      <c r="F11" s="12"/>
-      <c r="G11" s="12"/>
-      <c r="H11" s="12"/>
-      <c r="I11" s="12"/>
-    </row>
-    <row r="12" spans="1:9" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="13" t="s">
-        <v>5</v>
-      </c>
+      <c r="L10" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="M10" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="N10" s="12">
+        <v>18496</v>
+      </c>
+      <c r="O10" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="S10" s="11"/>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A11" s="17"/>
+      <c r="B11" s="6"/>
+      <c r="C11" s="9"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="10"/>
+      <c r="F11" s="10"/>
+      <c r="G11" s="10"/>
+      <c r="H11" s="10"/>
+      <c r="I11" s="10"/>
+      <c r="L11" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="M11" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="N11" s="14">
+        <v>0</v>
+      </c>
+      <c r="O11" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="S11" s="11"/>
+    </row>
+    <row r="12" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L12" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="M12" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="N12" s="12">
+        <v>73856</v>
+      </c>
+      <c r="O12" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="S12" s="11"/>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="L13" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="M13" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="N13" s="12">
+        <v>0</v>
+      </c>
+      <c r="O13" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="S13" s="11"/>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="L14" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="M14" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="N14" s="15">
+        <v>0</v>
+      </c>
+      <c r="O14" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="S14" s="11"/>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="B15" s="12"/>
+      <c r="L15" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="M15" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="N15" s="15">
+        <v>0</v>
+      </c>
+      <c r="O15" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="S15" s="11"/>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="B16" s="12"/>
+      <c r="L16" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="M16" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="N16" s="14">
+        <v>0</v>
+      </c>
+      <c r="O16" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="S16" s="11"/>
+    </row>
+    <row r="17" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="B17" s="12"/>
+      <c r="L17" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="M17" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="N17" s="12">
+        <v>409728</v>
+      </c>
+      <c r="O17" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="S17" s="11"/>
+    </row>
+    <row r="18" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="B18" s="12"/>
+      <c r="L18" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="M18" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="N18" s="12">
+        <v>0</v>
+      </c>
+      <c r="O18" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="S18" s="11"/>
+    </row>
+    <row r="19" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="B19" s="12"/>
+      <c r="L19" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="M19" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="N19" s="14">
+        <v>0</v>
+      </c>
+      <c r="O19" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="S19" s="11"/>
+    </row>
+    <row r="20" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="B20" s="12"/>
+      <c r="L20" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="M20" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="N20" s="12">
+        <v>1290</v>
+      </c>
+      <c r="O20" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="S20" s="11"/>
+    </row>
+    <row r="21" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+      <c r="F21" s="1"/>
+      <c r="G21" s="1"/>
+      <c r="L21" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="M21" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="N21" s="12">
+        <v>0</v>
+      </c>
+      <c r="O21" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="S21" s="11"/>
+    </row>
+    <row r="22" spans="2:19" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J22" s="11"/>
+      <c r="K22" s="11"/>
+      <c r="L22" s="13"/>
+      <c r="M22" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="N22" s="13">
+        <v>508458</v>
+      </c>
+      <c r="O22" s="13"/>
+      <c r="S22" s="11"/>
+    </row>
+    <row r="23" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="G23" s="1"/>
+      <c r="H23" s="1"/>
+      <c r="I23" s="1"/>
+      <c r="J23" s="11"/>
+      <c r="K23" s="11"/>
+      <c r="S23" s="11"/>
+    </row>
+    <row r="24" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+      <c r="F24" s="1"/>
+      <c r="G24" s="1"/>
+      <c r="H24" s="1"/>
+      <c r="I24" s="1"/>
+      <c r="J24" s="11"/>
+      <c r="K24" s="11"/>
+      <c r="S24" s="11"/>
+    </row>
+    <row r="25" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
+      <c r="F25" s="1"/>
+      <c r="G25" s="1"/>
+      <c r="H25" s="1"/>
+      <c r="I25" s="1"/>
+      <c r="J25" s="11"/>
+      <c r="K25" s="11"/>
+      <c r="S25" s="11"/>
+    </row>
+    <row r="26" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="J26" s="11"/>
+      <c r="K26" s="11"/>
+      <c r="S26" s="11"/>
+    </row>
+    <row r="27" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="J27" s="11"/>
+      <c r="K27" s="11"/>
+      <c r="S27" s="11"/>
+    </row>
+    <row r="28" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="J28" s="11"/>
+      <c r="K28" s="11"/>
+      <c r="S28" s="11"/>
+    </row>
+    <row r="29" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="J29" s="11"/>
+      <c r="K29" s="11"/>
+      <c r="S29" s="11"/>
+    </row>
+    <row r="30" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="J30" s="11"/>
+      <c r="K30" s="11"/>
+      <c r="S30" s="11"/>
+    </row>
+    <row r="31" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="J31" s="11"/>
+      <c r="K31" s="11"/>
+    </row>
+    <row r="32" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="J32" s="11"/>
+      <c r="K32" s="11"/>
+      <c r="P32" s="12"/>
+      <c r="Q32" s="12"/>
+      <c r="R32" s="12"/>
+      <c r="S32" s="11"/>
+    </row>
+    <row r="33" spans="10:19" x14ac:dyDescent="0.2">
+      <c r="J33" s="11"/>
+      <c r="K33" s="11"/>
+      <c r="S33" s="11"/>
+    </row>
+    <row r="34" spans="10:19" x14ac:dyDescent="0.2">
+      <c r="J34" s="11"/>
+      <c r="K34" s="11"/>
+      <c r="P34" s="12"/>
+      <c r="Q34" s="12"/>
+      <c r="R34" s="12"/>
+      <c r="S34" s="11"/>
+    </row>
+    <row r="35" spans="10:19" x14ac:dyDescent="0.2">
+      <c r="J35" s="11"/>
+      <c r="K35" s="11"/>
+      <c r="P35" s="12"/>
+      <c r="Q35" s="12"/>
+      <c r="R35" s="12"/>
+    </row>
+    <row r="36" spans="10:19" x14ac:dyDescent="0.2">
+      <c r="J36" s="11"/>
+      <c r="K36" s="11"/>
+      <c r="P36" s="12"/>
+      <c r="Q36" s="12"/>
+      <c r="R36" s="12"/>
+    </row>
+    <row r="37" spans="10:19" x14ac:dyDescent="0.2">
+      <c r="J37" s="11"/>
+      <c r="K37" s="11"/>
+      <c r="P37" s="12"/>
+      <c r="Q37" s="12"/>
+      <c r="R37" s="12"/>
+    </row>
+    <row r="38" spans="10:19" x14ac:dyDescent="0.2">
+      <c r="J38" s="11"/>
+      <c r="K38" s="11"/>
+      <c r="P38" s="12"/>
+      <c r="Q38" s="12"/>
+      <c r="R38" s="12"/>
+    </row>
+    <row r="39" spans="10:19" x14ac:dyDescent="0.2">
+      <c r="J39" s="11"/>
+      <c r="K39" s="11"/>
+      <c r="P39" s="12"/>
+      <c r="Q39" s="12"/>
+      <c r="R39" s="12"/>
+    </row>
+    <row r="40" spans="10:19" x14ac:dyDescent="0.2">
+      <c r="J40" s="11"/>
+      <c r="K40" s="11"/>
+      <c r="P40" s="12"/>
+      <c r="Q40" s="12"/>
+      <c r="R40" s="12"/>
+    </row>
+    <row r="41" spans="10:19" x14ac:dyDescent="0.2">
+      <c r="J41" s="11"/>
+      <c r="K41" s="11"/>
+      <c r="P41" s="12"/>
+      <c r="Q41" s="12"/>
+      <c r="R41" s="12"/>
+    </row>
+    <row r="42" spans="10:19" x14ac:dyDescent="0.2">
+      <c r="J42" s="11"/>
+      <c r="K42" s="11"/>
+      <c r="P42" s="12"/>
+      <c r="Q42" s="12"/>
+      <c r="R42" s="12"/>
+    </row>
+    <row r="43" spans="10:19" x14ac:dyDescent="0.2">
+      <c r="J43" s="11"/>
+      <c r="K43" s="11"/>
+      <c r="P43" s="12"/>
+      <c r="Q43" s="12"/>
+      <c r="R43" s="12"/>
+    </row>
+    <row r="44" spans="10:19" x14ac:dyDescent="0.2">
+      <c r="J44" s="11"/>
+      <c r="K44" s="11"/>
+      <c r="P44" s="12"/>
+      <c r="Q44" s="12"/>
+      <c r="R44" s="12"/>
+    </row>
+    <row r="45" spans="10:19" x14ac:dyDescent="0.2">
+      <c r="J45" s="11"/>
+      <c r="K45" s="11"/>
+      <c r="P45" s="12"/>
+      <c r="Q45" s="12"/>
+      <c r="R45" s="12"/>
+    </row>
+    <row r="46" spans="10:19" x14ac:dyDescent="0.2">
+      <c r="J46" s="11"/>
+      <c r="K46" s="11"/>
+      <c r="P46" s="12"/>
+      <c r="Q46" s="12"/>
+      <c r="R46" s="12"/>
+    </row>
+    <row r="47" spans="10:19" x14ac:dyDescent="0.2">
+      <c r="J47" s="11"/>
+      <c r="K47" s="11"/>
+      <c r="P47" s="12"/>
+      <c r="Q47" s="12"/>
+      <c r="R47" s="12"/>
+    </row>
+    <row r="48" spans="10:19" x14ac:dyDescent="0.2">
+      <c r="J48" s="11"/>
+      <c r="K48" s="11"/>
+      <c r="P48" s="12"/>
+      <c r="Q48" s="12"/>
+      <c r="R48" s="12"/>
+    </row>
+    <row r="49" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="J49" s="11"/>
+      <c r="K49" s="11"/>
+      <c r="P49" s="12"/>
+      <c r="Q49" s="12"/>
+      <c r="R49" s="12"/>
+    </row>
+    <row r="50" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="J50" s="11"/>
+      <c r="K50" s="11"/>
+      <c r="P50" s="12"/>
+      <c r="Q50" s="12"/>
+      <c r="R50" s="12"/>
+    </row>
+    <row r="51" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B51" s="11"/>
+      <c r="C51" s="11"/>
+      <c r="D51" s="11"/>
+      <c r="E51" s="11"/>
+      <c r="F51" s="11"/>
+      <c r="G51" s="11"/>
+      <c r="H51" s="11"/>
+      <c r="I51" s="11"/>
+      <c r="J51" s="11"/>
+      <c r="K51" s="11"/>
+      <c r="P51" s="12"/>
+      <c r="Q51" s="12"/>
+      <c r="R51" s="12"/>
+    </row>
+    <row r="52" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B52" s="11"/>
+      <c r="C52" s="11"/>
+      <c r="D52" s="11"/>
+      <c r="E52" s="11"/>
+      <c r="F52" s="11"/>
+      <c r="G52" s="11"/>
+      <c r="H52" s="11"/>
+      <c r="I52" s="11"/>
+      <c r="J52" s="11"/>
+      <c r="K52" s="11"/>
+      <c r="P52" s="12"/>
+      <c r="Q52" s="12"/>
+      <c r="R52" s="12"/>
+    </row>
+    <row r="53" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B53" s="11"/>
+      <c r="C53" s="11"/>
+      <c r="D53" s="11"/>
+      <c r="E53" s="11"/>
+      <c r="F53" s="11"/>
+      <c r="G53" s="11"/>
+      <c r="H53" s="11"/>
+      <c r="I53" s="11"/>
+      <c r="J53" s="11"/>
+      <c r="K53" s="11"/>
+      <c r="P53" s="12"/>
+      <c r="Q53" s="12"/>
+      <c r="R53" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="C3:I3"/>
-    <mergeCell ref="A5:A11"/>
+    <mergeCell ref="A5:A10"/>
+    <mergeCell ref="C3:G3"/>
   </mergeCells>
-  <conditionalFormatting sqref="C5:G9 C11:I11">
+  <conditionalFormatting sqref="C11:I11">
+    <cfRule type="colorScale" priority="6">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C11:I11">
+    <cfRule type="colorScale" priority="7">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C11:I11 H9:I10">
+    <cfRule type="colorScale" priority="5">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H9:I10">
+    <cfRule type="colorScale" priority="4">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H5:I9">
     <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="min"/>
@@ -967,19 +2094,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C7:G9 C11:I11">
-    <cfRule type="colorScale" priority="4">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C5:I11">
+  <conditionalFormatting sqref="C5:G9 C10:D10 G10">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
@@ -991,7 +2106,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C5:I10">
+  <conditionalFormatting sqref="C5:G10">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
@@ -1029,13 +2144,13 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="C4" s="9" t="s">
+      <c r="C4" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="9"/>
-      <c r="E4" s="9"/>
-      <c r="F4" s="9"/>
-      <c r="G4" s="9"/>
+      <c r="D4" s="19"/>
+      <c r="E4" s="19"/>
+      <c r="F4" s="19"/>
+      <c r="G4" s="19"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C5" s="2">
@@ -1055,7 +2170,7 @@
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6" s="10" t="s">
+      <c r="A6" s="20" t="s">
         <v>1</v>
       </c>
       <c r="B6" s="2">
@@ -1078,7 +2193,7 @@
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A7" s="10"/>
+      <c r="A7" s="20"/>
       <c r="B7" s="2">
         <v>8</v>
       </c>
@@ -1099,7 +2214,7 @@
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A8" s="10"/>
+      <c r="A8" s="20"/>
       <c r="B8" s="2">
         <v>16</v>
       </c>
@@ -1120,7 +2235,7 @@
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A9" s="10"/>
+      <c r="A9" s="20"/>
       <c r="B9" s="2">
         <v>32</v>
       </c>
@@ -1141,7 +2256,7 @@
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A10" s="10"/>
+      <c r="A10" s="20"/>
       <c r="B10" s="2">
         <v>64</v>
       </c>

</xml_diff>

<commit_message>
Add new networks; Do MNIST
</commit_message>
<xml_diff>
--- a/resultats/cnn_gridsearch.xlsx
+++ b/resultats/cnn_gridsearch.xlsx
@@ -9,16 +9,21 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="860" yWindow="440" windowWidth="26140" windowHeight="17560" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="1600" yWindow="560" windowWidth="26140" windowHeight="17560" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="MNIST-CNN1" sheetId="2" r:id="rId1"/>
     <sheet name="CIFAR10-CNN1" sheetId="3" r:id="rId2"/>
-    <sheet name="Essai" sheetId="1" r:id="rId3"/>
+    <sheet name="MNIST-CNN2" sheetId="5" r:id="rId3"/>
+    <sheet name="CIFAR10-CNN2" sheetId="4" r:id="rId4"/>
+    <sheet name="Essai" sheetId="1" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="gridsearch" localSheetId="2">Essai!$C$6:$G$10</definedName>
+    <definedName name="gridsearch" localSheetId="3">'CIFAR10-CNN2'!$C$5:$E$9</definedName>
+    <definedName name="gridsearch" localSheetId="4">Essai!$C$6:$G$10</definedName>
+    <definedName name="gridsearch" localSheetId="2">'MNIST-CNN2'!$C$5:$E$9</definedName>
     <definedName name="gridsearch_1" localSheetId="1">'CIFAR10-CNN1'!$C$19:$H$25</definedName>
+    <definedName name="gridsearch_1" localSheetId="3">'CIFAR10-CNN2'!$C$25:$E$29</definedName>
     <definedName name="gridsearch_1" localSheetId="0">'MNIST-CNN1'!$C$5:$G$9</definedName>
     <definedName name="gridsearch_2" localSheetId="1">'CIFAR10-CNN1'!$C$5:$G$10</definedName>
   </definedNames>
@@ -58,7 +63,25 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="3" name="gridsearch3" type="6" refreshedVersion="0" background="1" saveData="1">
+  <connection id="3" name="gridsearch2" type="6" refreshedVersion="0" background="1" saveData="1">
+    <textPr fileType="mac" sourceFile="/Users/carl/Documents/uni/RecFormesAnalyseIm/Analyse_dimage_avance_proj/gridsearch.csv" thousands=" ">
+      <textFields count="3">
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="4" name="gridsearch21" type="6" refreshedVersion="0" background="1" saveData="1">
+    <textPr fileType="mac" sourceFile="/Users/carl/Documents/uni/RecFormesAnalyseIm/Analyse_dimage_avance_proj/gridsearch.csv" thousands=" ">
+      <textFields count="3">
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="5" name="gridsearch3" type="6" refreshedVersion="0" background="1" saveData="1">
     <textPr fileType="mac" sourceFile="/Users/carl/Documents/uni/RecFormesAnalyseIm/Analyse_dimage_avance_proj/gridsearch.csv" thousands=" ">
       <textFields count="7">
         <textField/>
@@ -71,11 +94,20 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="4" name="gridsearch4" type="6" refreshedVersion="0" background="1" saveData="1">
-    <textPr fileType="mac" codePage="10000" sourceFile="/Users/carl/Documents/uni/RecFormesAnalyseIm/Analyse_dimage_avance_proj/gridsearch.csv" thousands=" ">
+  <connection id="6" name="gridsearch4" type="6" refreshedVersion="0" background="1" saveData="1">
+    <textPr fileType="mac" sourceFile="/Users/carl/Documents/uni/RecFormesAnalyseIm/Analyse_dimage_avance_proj/gridsearch.csv" thousands=" ">
       <textFields count="5">
         <textField/>
         <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="7" name="gridsearch5" type="6" refreshedVersion="0" background="1" saveData="1">
+    <textPr fileType="mac" codePage="10000" sourceFile="/Users/carl/Documents/uni/RecFormesAnalyseIm/Analyse_dimage_avance_proj/gridsearch.csv" thousands=" ">
+      <textFields count="3">
         <textField/>
         <textField/>
         <textField/>
@@ -86,7 +118,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="113">
   <si>
     <t>Batch size</t>
   </si>
@@ -432,6 +464,150 @@
   </si>
   <si>
     <t>Refaire car persistence des poids</t>
+  </si>
+  <si>
+    <t>convolution2d_13 (Convolution2D)</t>
+  </si>
+  <si>
+    <t>(None, 30, 30, 64)</t>
+  </si>
+  <si>
+    <t>convolution2d_input_5[0][0]</t>
+  </si>
+  <si>
+    <t>activation_21 (Activation)</t>
+  </si>
+  <si>
+    <t>convolution2d_13[0][0]</t>
+  </si>
+  <si>
+    <t>dropout_9 (Dropout)</t>
+  </si>
+  <si>
+    <t>activation_21[0][0]</t>
+  </si>
+  <si>
+    <t>convolution2d_14 (Convolution2D)</t>
+  </si>
+  <si>
+    <t>(None, 28, 28, 64)</t>
+  </si>
+  <si>
+    <t>dropout_9[0][0]</t>
+  </si>
+  <si>
+    <t>activation_22 (Activation)</t>
+  </si>
+  <si>
+    <t>convolution2d_14[0][0]</t>
+  </si>
+  <si>
+    <t>maxpooling2d_9 (MaxPooling2D)</t>
+  </si>
+  <si>
+    <t>(None, 14, 14, 64)</t>
+  </si>
+  <si>
+    <t>activation_22[0][0]</t>
+  </si>
+  <si>
+    <t>convolution2d_15 (Convolution2D)</t>
+  </si>
+  <si>
+    <t>(None, 12, 12, 128)</t>
+  </si>
+  <si>
+    <t>maxpooling2d_9[0][0]</t>
+  </si>
+  <si>
+    <t>activation_23 (Activation)</t>
+  </si>
+  <si>
+    <t>convolution2d_15[0][0]</t>
+  </si>
+  <si>
+    <t>maxpooling2d_10 (MaxPooling2D)</t>
+  </si>
+  <si>
+    <t>(None, 6, 6, 128)</t>
+  </si>
+  <si>
+    <t>activation_23[0][0]</t>
+  </si>
+  <si>
+    <t>flatten_5 (Flatten)</t>
+  </si>
+  <si>
+    <t>(None, 4608)</t>
+  </si>
+  <si>
+    <t>maxpooling2d_10[0][0]</t>
+  </si>
+  <si>
+    <t>dense_9 (Dense)</t>
+  </si>
+  <si>
+    <t>(None, 512)</t>
+  </si>
+  <si>
+    <t>flatten_5[0][0]</t>
+  </si>
+  <si>
+    <t>activation_24 (Activation)</t>
+  </si>
+  <si>
+    <t>dense_9[0][0]</t>
+  </si>
+  <si>
+    <t>dropout_10 (Dropout)</t>
+  </si>
+  <si>
+    <t>activation_24[0][0]</t>
+  </si>
+  <si>
+    <t>dense_10 (Dense)</t>
+  </si>
+  <si>
+    <t>dropout_10[0][0]</t>
+  </si>
+  <si>
+    <t>activation_25 (Activation)</t>
+  </si>
+  <si>
+    <t>dense_10[0][0]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total params: </t>
+  </si>
+  <si>
+    <t>Num. neurons in dense layer</t>
+  </si>
+  <si>
+    <t>Exemple de réseau:</t>
+  </si>
+  <si>
+    <t>Epochs: 10</t>
+  </si>
+  <si>
+    <t>10 epochs</t>
+  </si>
+  <si>
+    <t>(None, 26, 26, 64)</t>
+  </si>
+  <si>
+    <t>(None, 24, 24, 64)</t>
+  </si>
+  <si>
+    <t>(None, 12, 12, 64)</t>
+  </si>
+  <si>
+    <t>(None, 10, 10, 128)</t>
+  </si>
+  <si>
+    <t>(None, 5, 5, 128)</t>
+  </si>
+  <si>
+    <t>Total params</t>
   </si>
 </sst>
 </file>
@@ -496,7 +672,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -521,8 +697,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF9696B"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -554,8 +736,65 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="double">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="51">
+  <cellStyleXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -607,8 +846,20 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -637,13 +888,37 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="10" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="51">
+  <cellStyles count="63">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="5" builtinId="8" hidden="1"/>
@@ -669,6 +944,12 @@
     <cellStyle name="Lien hypertexte" xfId="45" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="47" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="61" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="6" builtinId="9" hidden="1"/>
@@ -694,10 +975,21 @@
     <cellStyle name="Lien hypertexte visité" xfId="46" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="48" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="62" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFF9696B"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -711,14 +1003,26 @@
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="gridsearch_2" connectionId="4" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="gridsearch_2" connectionId="6" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="gridsearch_1" connectionId="3" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="gridsearch_1" connectionId="5" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="gridsearch" connectionId="7" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable5.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="gridsearch_1" connectionId="4" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable6.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="gridsearch" connectionId="3" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable7.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="gridsearch" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
@@ -1002,15 +1306,15 @@
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="C3" s="19" t="s">
-        <v>0</v>
-      </c>
-      <c r="D3" s="19"/>
-      <c r="E3" s="19"/>
-      <c r="F3" s="19"/>
-      <c r="G3" s="19"/>
-      <c r="H3" s="19"/>
-      <c r="I3" s="19"/>
+      <c r="C3" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" s="29"/>
+      <c r="E3" s="29"/>
+      <c r="F3" s="29"/>
+      <c r="G3" s="29"/>
+      <c r="H3" s="29"/>
+      <c r="I3" s="29"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C4" s="2">
@@ -1036,7 +1340,7 @@
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A5" s="20" t="s">
+      <c r="A5" s="30" t="s">
         <v>1</v>
       </c>
       <c r="B5" s="2">
@@ -1065,7 +1369,7 @@
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A6" s="20"/>
+      <c r="A6" s="30"/>
       <c r="B6" s="2">
         <v>8</v>
       </c>
@@ -1092,7 +1396,7 @@
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A7" s="20"/>
+      <c r="A7" s="30"/>
       <c r="B7" s="2">
         <v>16</v>
       </c>
@@ -1119,7 +1423,7 @@
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A8" s="20"/>
+      <c r="A8" s="30"/>
       <c r="B8" s="2">
         <v>32</v>
       </c>
@@ -1146,7 +1450,7 @@
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A9" s="20"/>
+      <c r="A9" s="30"/>
       <c r="B9" s="2">
         <v>64</v>
       </c>
@@ -1173,7 +1477,7 @@
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A10" s="20"/>
+      <c r="A10" s="30"/>
       <c r="B10" s="5">
         <v>128</v>
       </c>
@@ -1200,7 +1504,7 @@
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A11" s="20"/>
+      <c r="A11" s="30"/>
       <c r="B11" s="5">
         <v>256</v>
       </c>
@@ -1220,15 +1524,15 @@
       <c r="B12" s="6"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A13" s="22" t="s">
+      <c r="A13" s="21" t="s">
         <v>64</v>
       </c>
-      <c r="B13" s="22"/>
-      <c r="C13" s="22"/>
-      <c r="D13" s="22"/>
-      <c r="E13" s="22"/>
-      <c r="F13" s="22"/>
-      <c r="G13" s="22"/>
+      <c r="B13" s="21"/>
+      <c r="C13" s="21"/>
+      <c r="D13" s="21"/>
+      <c r="E13" s="21"/>
+      <c r="F13" s="21"/>
+      <c r="G13" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -1284,15 +1588,16 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P53"/>
+  <dimension ref="A1:P64"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+    <sheetView zoomScale="92" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1324,14 +1629,14 @@
       <c r="O2" s="12"/>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="C3" s="19" t="s">
-        <v>0</v>
-      </c>
-      <c r="D3" s="19"/>
-      <c r="E3" s="19"/>
-      <c r="F3" s="19"/>
-      <c r="G3" s="19"/>
-      <c r="H3" s="21"/>
+      <c r="C3" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" s="29"/>
+      <c r="E3" s="29"/>
+      <c r="F3" s="29"/>
+      <c r="G3" s="29"/>
+      <c r="H3" s="20"/>
       <c r="I3" s="13" t="s">
         <v>4</v>
       </c>
@@ -1376,7 +1681,7 @@
       </c>
     </row>
     <row r="5" spans="1:16" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="20" t="s">
+      <c r="A5" s="30" t="s">
         <v>63</v>
       </c>
       <c r="B5" s="2" t="s">
@@ -1412,7 +1717,7 @@
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A6" s="20"/>
+      <c r="A6" s="30"/>
       <c r="B6" s="2" t="s">
         <v>57</v>
       </c>
@@ -1447,7 +1752,7 @@
       <c r="P6" s="11"/>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A7" s="20"/>
+      <c r="A7" s="30"/>
       <c r="B7" s="2" t="s">
         <v>58</v>
       </c>
@@ -1482,7 +1787,7 @@
       <c r="P7" s="11"/>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A8" s="20"/>
+      <c r="A8" s="30"/>
       <c r="B8" s="2" t="s">
         <v>59</v>
       </c>
@@ -1517,7 +1822,7 @@
       <c r="P8" s="11"/>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A9" s="20"/>
+      <c r="A9" s="30"/>
       <c r="B9" s="2" t="s">
         <v>60</v>
       </c>
@@ -1552,7 +1857,7 @@
       <c r="P9" s="11"/>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A10" s="20"/>
+      <c r="A10" s="30"/>
       <c r="B10" s="2" t="s">
         <v>61</v>
       </c>
@@ -1824,99 +2129,111 @@
       <c r="O32" s="12"/>
       <c r="P32" s="11"/>
     </row>
-    <row r="33" spans="13:16" x14ac:dyDescent="0.2">
+    <row r="33" spans="3:16" x14ac:dyDescent="0.2">
       <c r="P33" s="11"/>
     </row>
-    <row r="34" spans="13:16" x14ac:dyDescent="0.2">
+    <row r="34" spans="3:16" x14ac:dyDescent="0.2">
       <c r="M34" s="12"/>
       <c r="N34" s="12"/>
       <c r="O34" s="12"/>
       <c r="P34" s="11"/>
     </row>
-    <row r="35" spans="13:16" x14ac:dyDescent="0.2">
+    <row r="35" spans="3:16" x14ac:dyDescent="0.2">
       <c r="M35" s="12"/>
       <c r="N35" s="12"/>
       <c r="O35" s="12"/>
     </row>
-    <row r="36" spans="13:16" x14ac:dyDescent="0.2">
+    <row r="36" spans="3:16" x14ac:dyDescent="0.2">
       <c r="M36" s="12"/>
       <c r="N36" s="12"/>
       <c r="O36" s="12"/>
     </row>
-    <row r="37" spans="13:16" x14ac:dyDescent="0.2">
+    <row r="37" spans="3:16" x14ac:dyDescent="0.2">
       <c r="M37" s="12"/>
       <c r="N37" s="12"/>
       <c r="O37" s="12"/>
     </row>
-    <row r="38" spans="13:16" x14ac:dyDescent="0.2">
+    <row r="38" spans="3:16" x14ac:dyDescent="0.2">
       <c r="M38" s="12"/>
       <c r="N38" s="12"/>
       <c r="O38" s="12"/>
     </row>
-    <row r="39" spans="13:16" x14ac:dyDescent="0.2">
+    <row r="39" spans="3:16" x14ac:dyDescent="0.2">
       <c r="M39" s="12"/>
       <c r="N39" s="12"/>
       <c r="O39" s="12"/>
     </row>
-    <row r="40" spans="13:16" x14ac:dyDescent="0.2">
+    <row r="40" spans="3:16" x14ac:dyDescent="0.2">
       <c r="M40" s="12"/>
       <c r="N40" s="12"/>
       <c r="O40" s="12"/>
     </row>
-    <row r="41" spans="13:16" x14ac:dyDescent="0.2">
+    <row r="41" spans="3:16" x14ac:dyDescent="0.2">
       <c r="M41" s="12"/>
       <c r="N41" s="12"/>
       <c r="O41" s="12"/>
     </row>
-    <row r="42" spans="13:16" x14ac:dyDescent="0.2">
+    <row r="42" spans="3:16" x14ac:dyDescent="0.2">
       <c r="M42" s="12"/>
       <c r="N42" s="12"/>
       <c r="O42" s="12"/>
     </row>
-    <row r="43" spans="13:16" x14ac:dyDescent="0.2">
+    <row r="43" spans="3:16" x14ac:dyDescent="0.2">
       <c r="M43" s="12"/>
       <c r="N43" s="12"/>
       <c r="O43" s="12"/>
     </row>
-    <row r="44" spans="13:16" x14ac:dyDescent="0.2">
+    <row r="44" spans="3:16" x14ac:dyDescent="0.2">
       <c r="M44" s="12"/>
       <c r="N44" s="12"/>
       <c r="O44" s="12"/>
     </row>
-    <row r="45" spans="13:16" x14ac:dyDescent="0.2">
+    <row r="45" spans="3:16" x14ac:dyDescent="0.2">
+      <c r="C45" s="12"/>
+      <c r="D45" s="12"/>
       <c r="M45" s="12"/>
       <c r="N45" s="12"/>
       <c r="O45" s="12"/>
     </row>
-    <row r="46" spans="13:16" x14ac:dyDescent="0.2">
+    <row r="46" spans="3:16" x14ac:dyDescent="0.2">
+      <c r="C46" s="12"/>
+      <c r="D46" s="12"/>
       <c r="M46" s="12"/>
       <c r="N46" s="12"/>
       <c r="O46" s="12"/>
     </row>
-    <row r="47" spans="13:16" x14ac:dyDescent="0.2">
+    <row r="47" spans="3:16" x14ac:dyDescent="0.2">
+      <c r="C47" s="12"/>
+      <c r="D47" s="12"/>
       <c r="M47" s="12"/>
       <c r="N47" s="12"/>
       <c r="O47" s="12"/>
     </row>
-    <row r="48" spans="13:16" x14ac:dyDescent="0.2">
+    <row r="48" spans="3:16" x14ac:dyDescent="0.2">
+      <c r="C48" s="12"/>
+      <c r="D48" s="12"/>
       <c r="M48" s="12"/>
       <c r="N48" s="12"/>
       <c r="O48" s="12"/>
     </row>
     <row r="49" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="C49" s="12"/>
+      <c r="D49" s="12"/>
       <c r="M49" s="12"/>
       <c r="N49" s="12"/>
       <c r="O49" s="12"/>
     </row>
     <row r="50" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="C50" s="12"/>
+      <c r="D50" s="12"/>
       <c r="M50" s="12"/>
       <c r="N50" s="12"/>
       <c r="O50" s="12"/>
     </row>
     <row r="51" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B51" s="11"/>
-      <c r="C51" s="11"/>
-      <c r="D51" s="11"/>
+      <c r="C51" s="12"/>
+      <c r="D51" s="12"/>
       <c r="E51" s="11"/>
       <c r="F51" s="11"/>
       <c r="G51" s="11"/>
@@ -1927,8 +2244,8 @@
     </row>
     <row r="52" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B52" s="11"/>
-      <c r="C52" s="11"/>
-      <c r="D52" s="11"/>
+      <c r="C52" s="12"/>
+      <c r="D52" s="12"/>
       <c r="E52" s="11"/>
       <c r="F52" s="11"/>
       <c r="G52" s="11"/>
@@ -1939,8 +2256,8 @@
     </row>
     <row r="53" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B53" s="11"/>
-      <c r="C53" s="11"/>
-      <c r="D53" s="11"/>
+      <c r="C53" s="12"/>
+      <c r="D53" s="12"/>
       <c r="E53" s="11"/>
       <c r="F53" s="11"/>
       <c r="G53" s="11"/>
@@ -1948,6 +2265,46 @@
       <c r="M53" s="12"/>
       <c r="N53" s="12"/>
       <c r="O53" s="12"/>
+    </row>
+    <row r="54" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="C54" s="12"/>
+      <c r="D54" s="12"/>
+    </row>
+    <row r="55" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="C55" s="12"/>
+      <c r="D55" s="12"/>
+    </row>
+    <row r="56" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="C56" s="12"/>
+      <c r="D56" s="12"/>
+    </row>
+    <row r="57" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="C57" s="12"/>
+      <c r="D57" s="12"/>
+    </row>
+    <row r="58" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="C58" s="12"/>
+      <c r="D58" s="12"/>
+    </row>
+    <row r="59" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="C59" s="12"/>
+      <c r="D59" s="12"/>
+    </row>
+    <row r="60" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="C60" s="12"/>
+      <c r="D60" s="12"/>
+    </row>
+    <row r="61" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="C61" s="12"/>
+    </row>
+    <row r="62" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="C62" s="12"/>
+    </row>
+    <row r="63" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="C63" s="12"/>
+    </row>
+    <row r="64" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="C64" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -2032,6 +2389,828 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G26" sqref="G26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="5.6640625" customWidth="1"/>
+    <col min="3" max="5" width="8.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="31.33203125" customWidth="1"/>
+    <col min="8" max="8" width="18.5" customWidth="1"/>
+    <col min="9" max="9" width="8.83203125" customWidth="1"/>
+    <col min="10" max="10" width="26.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="G2" s="34" t="s">
+        <v>4</v>
+      </c>
+      <c r="H2" s="34" t="s">
+        <v>5</v>
+      </c>
+      <c r="I2" s="34" t="s">
+        <v>6</v>
+      </c>
+      <c r="J2" s="34" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="C3" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" s="29"/>
+      <c r="E3" s="29"/>
+      <c r="G3" t="s">
+        <v>65</v>
+      </c>
+      <c r="H3" t="s">
+        <v>107</v>
+      </c>
+      <c r="I3">
+        <v>640</v>
+      </c>
+      <c r="J3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="C4" s="22">
+        <v>32</v>
+      </c>
+      <c r="D4" s="22">
+        <v>128</v>
+      </c>
+      <c r="E4" s="22">
+        <v>512</v>
+      </c>
+      <c r="G4" t="s">
+        <v>68</v>
+      </c>
+      <c r="H4" t="s">
+        <v>107</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
+      </c>
+      <c r="J4" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A5" s="30" t="s">
+        <v>103</v>
+      </c>
+      <c r="B5" s="2">
+        <v>32</v>
+      </c>
+      <c r="C5" s="1">
+        <v>0.99170000000000003</v>
+      </c>
+      <c r="D5" s="1">
+        <v>0.99180000000000001</v>
+      </c>
+      <c r="E5" s="1">
+        <v>0.98780000000000001</v>
+      </c>
+      <c r="G5" s="25" t="s">
+        <v>70</v>
+      </c>
+      <c r="H5" s="25" t="s">
+        <v>107</v>
+      </c>
+      <c r="I5" s="25">
+        <v>0</v>
+      </c>
+      <c r="J5" s="25" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A6" s="30"/>
+      <c r="B6" s="2">
+        <v>64</v>
+      </c>
+      <c r="C6" s="1">
+        <v>0.99360000000000004</v>
+      </c>
+      <c r="D6" s="1">
+        <v>0.99109999999999898</v>
+      </c>
+      <c r="E6" s="1">
+        <v>0.99180000000000001</v>
+      </c>
+      <c r="G6" t="s">
+        <v>72</v>
+      </c>
+      <c r="H6" t="s">
+        <v>108</v>
+      </c>
+      <c r="I6">
+        <v>36928</v>
+      </c>
+      <c r="J6" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A7" s="30"/>
+      <c r="B7" s="2">
+        <v>128</v>
+      </c>
+      <c r="C7" s="1">
+        <v>0.9929</v>
+      </c>
+      <c r="D7" s="1">
+        <v>0.99339999999999895</v>
+      </c>
+      <c r="E7" s="1">
+        <v>0.99229999999999896</v>
+      </c>
+      <c r="G7" t="s">
+        <v>75</v>
+      </c>
+      <c r="H7" t="s">
+        <v>108</v>
+      </c>
+      <c r="I7">
+        <v>0</v>
+      </c>
+      <c r="J7" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A8" s="30"/>
+      <c r="B8" s="2">
+        <v>256</v>
+      </c>
+      <c r="C8" s="1">
+        <v>0.99209999999999898</v>
+      </c>
+      <c r="D8" s="1">
+        <v>0.99350000000000005</v>
+      </c>
+      <c r="E8" s="1">
+        <v>0.99239999999999895</v>
+      </c>
+      <c r="G8" s="25" t="s">
+        <v>77</v>
+      </c>
+      <c r="H8" s="25" t="s">
+        <v>109</v>
+      </c>
+      <c r="I8" s="25">
+        <v>0</v>
+      </c>
+      <c r="J8" s="25" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A9" s="30"/>
+      <c r="B9" s="2">
+        <v>512</v>
+      </c>
+      <c r="C9" s="1">
+        <v>0.9919</v>
+      </c>
+      <c r="D9" s="1">
+        <v>0.99409999999999898</v>
+      </c>
+      <c r="E9" s="1">
+        <v>0.99390000000000001</v>
+      </c>
+      <c r="G9" t="s">
+        <v>80</v>
+      </c>
+      <c r="H9" t="s">
+        <v>110</v>
+      </c>
+      <c r="I9">
+        <v>73856</v>
+      </c>
+      <c r="J9" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="G10" t="s">
+        <v>83</v>
+      </c>
+      <c r="H10" t="s">
+        <v>110</v>
+      </c>
+      <c r="I10">
+        <v>0</v>
+      </c>
+      <c r="J10" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="G11" t="s">
+        <v>85</v>
+      </c>
+      <c r="H11" t="s">
+        <v>111</v>
+      </c>
+      <c r="I11">
+        <v>0</v>
+      </c>
+      <c r="J11" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="G12" s="25" t="s">
+        <v>88</v>
+      </c>
+      <c r="H12" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="I12" s="25">
+        <v>0</v>
+      </c>
+      <c r="J12" s="25" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="G13" t="s">
+        <v>91</v>
+      </c>
+      <c r="H13" t="s">
+        <v>92</v>
+      </c>
+      <c r="I13">
+        <v>1638912</v>
+      </c>
+      <c r="J13" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="G14" t="s">
+        <v>94</v>
+      </c>
+      <c r="H14" t="s">
+        <v>92</v>
+      </c>
+      <c r="I14">
+        <v>0</v>
+      </c>
+      <c r="J14" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="G15" s="25" t="s">
+        <v>96</v>
+      </c>
+      <c r="H15" s="25" t="s">
+        <v>92</v>
+      </c>
+      <c r="I15" s="25">
+        <v>0</v>
+      </c>
+      <c r="J15" s="25" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="G16" t="s">
+        <v>98</v>
+      </c>
+      <c r="H16" t="s">
+        <v>43</v>
+      </c>
+      <c r="I16">
+        <v>5130</v>
+      </c>
+      <c r="J16" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="17" spans="7:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="G17" s="24" t="s">
+        <v>100</v>
+      </c>
+      <c r="H17" s="24" t="s">
+        <v>43</v>
+      </c>
+      <c r="I17" s="24">
+        <v>0</v>
+      </c>
+      <c r="J17" s="24" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="18" spans="7:10" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="H18" t="s">
+        <v>112</v>
+      </c>
+      <c r="I18">
+        <v>1755466</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="C3:E3"/>
+    <mergeCell ref="A5:A9"/>
+  </mergeCells>
+  <conditionalFormatting sqref="C5:E9">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L27"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="6" customWidth="1"/>
+    <col min="3" max="4" width="8.1640625" customWidth="1"/>
+    <col min="9" max="9" width="31.6640625" customWidth="1"/>
+    <col min="10" max="10" width="18.1640625" customWidth="1"/>
+    <col min="11" max="11" width="9.33203125" customWidth="1"/>
+    <col min="12" max="12" width="25.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>106</v>
+      </c>
+      <c r="I1" s="26" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C3" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" s="29"/>
+      <c r="E3" s="29"/>
+      <c r="I3" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="J3" s="23" t="s">
+        <v>5</v>
+      </c>
+      <c r="K3" s="23" t="s">
+        <v>6</v>
+      </c>
+      <c r="L3" s="23" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="C4" s="19">
+        <v>32</v>
+      </c>
+      <c r="D4" s="19">
+        <v>128</v>
+      </c>
+      <c r="E4" s="19">
+        <v>512</v>
+      </c>
+      <c r="I4" t="s">
+        <v>65</v>
+      </c>
+      <c r="J4" t="s">
+        <v>66</v>
+      </c>
+      <c r="K4">
+        <v>1792</v>
+      </c>
+      <c r="L4" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A5" s="30" t="s">
+        <v>103</v>
+      </c>
+      <c r="B5" s="2">
+        <v>32</v>
+      </c>
+      <c r="C5" s="1">
+        <v>0.5534</v>
+      </c>
+      <c r="D5" s="1">
+        <v>0.52180000000000004</v>
+      </c>
+      <c r="E5" s="1">
+        <v>0.55620000000000003</v>
+      </c>
+      <c r="I5" t="s">
+        <v>68</v>
+      </c>
+      <c r="J5" t="s">
+        <v>66</v>
+      </c>
+      <c r="K5">
+        <v>0</v>
+      </c>
+      <c r="L5" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A6" s="30"/>
+      <c r="B6" s="2">
+        <v>64</v>
+      </c>
+      <c r="C6" s="1">
+        <v>0.62729999999999897</v>
+      </c>
+      <c r="D6" s="1">
+        <v>0.64119999999999899</v>
+      </c>
+      <c r="E6" s="1">
+        <v>0.56559999999999899</v>
+      </c>
+      <c r="I6" s="25" t="s">
+        <v>70</v>
+      </c>
+      <c r="J6" s="25" t="s">
+        <v>66</v>
+      </c>
+      <c r="K6" s="25">
+        <v>0</v>
+      </c>
+      <c r="L6" s="25" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A7" s="30"/>
+      <c r="B7" s="2">
+        <v>128</v>
+      </c>
+      <c r="C7" s="1">
+        <v>0.66810000000000003</v>
+      </c>
+      <c r="D7" s="1">
+        <v>0.64910000000000001</v>
+      </c>
+      <c r="E7" s="1">
+        <v>0.60070000000000001</v>
+      </c>
+      <c r="I7" t="s">
+        <v>72</v>
+      </c>
+      <c r="J7" t="s">
+        <v>73</v>
+      </c>
+      <c r="K7">
+        <v>36928</v>
+      </c>
+      <c r="L7" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A8" s="30"/>
+      <c r="B8" s="2">
+        <v>256</v>
+      </c>
+      <c r="C8" s="1">
+        <v>0.67979999999999896</v>
+      </c>
+      <c r="D8" s="1">
+        <v>0.64970000000000006</v>
+      </c>
+      <c r="E8" s="1">
+        <v>0.61050000000000004</v>
+      </c>
+      <c r="I8" t="s">
+        <v>75</v>
+      </c>
+      <c r="J8" t="s">
+        <v>73</v>
+      </c>
+      <c r="K8">
+        <v>0</v>
+      </c>
+      <c r="L8" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A9" s="30"/>
+      <c r="B9" s="2">
+        <v>512</v>
+      </c>
+      <c r="C9" s="1">
+        <v>0.71589999999999898</v>
+      </c>
+      <c r="D9" s="27">
+        <v>0.1</v>
+      </c>
+      <c r="E9" s="1">
+        <v>0.63229999999999997</v>
+      </c>
+      <c r="I9" s="25" t="s">
+        <v>77</v>
+      </c>
+      <c r="J9" s="25" t="s">
+        <v>78</v>
+      </c>
+      <c r="K9" s="25">
+        <v>0</v>
+      </c>
+      <c r="L9" s="25" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="I10" t="s">
+        <v>80</v>
+      </c>
+      <c r="J10" t="s">
+        <v>81</v>
+      </c>
+      <c r="K10">
+        <v>73856</v>
+      </c>
+      <c r="L10" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="I11" t="s">
+        <v>83</v>
+      </c>
+      <c r="J11" t="s">
+        <v>81</v>
+      </c>
+      <c r="K11">
+        <v>0</v>
+      </c>
+      <c r="L11" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="I12" t="s">
+        <v>85</v>
+      </c>
+      <c r="J12" t="s">
+        <v>86</v>
+      </c>
+      <c r="K12">
+        <v>0</v>
+      </c>
+      <c r="L12" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I13" s="25" t="s">
+        <v>88</v>
+      </c>
+      <c r="J13" s="25" t="s">
+        <v>89</v>
+      </c>
+      <c r="K13" s="25">
+        <v>0</v>
+      </c>
+      <c r="L13" s="25" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="I14" t="s">
+        <v>91</v>
+      </c>
+      <c r="J14" t="s">
+        <v>92</v>
+      </c>
+      <c r="K14">
+        <v>2359808</v>
+      </c>
+      <c r="L14" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="I15" t="s">
+        <v>94</v>
+      </c>
+      <c r="J15" t="s">
+        <v>92</v>
+      </c>
+      <c r="K15">
+        <v>0</v>
+      </c>
+      <c r="L15" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="I16" s="25" t="s">
+        <v>96</v>
+      </c>
+      <c r="J16" s="25" t="s">
+        <v>92</v>
+      </c>
+      <c r="K16" s="25">
+        <v>0</v>
+      </c>
+      <c r="L16" s="25" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="I17" t="s">
+        <v>98</v>
+      </c>
+      <c r="J17" t="s">
+        <v>43</v>
+      </c>
+      <c r="K17">
+        <v>5130</v>
+      </c>
+      <c r="L17" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="I18" s="24" t="s">
+        <v>100</v>
+      </c>
+      <c r="J18" s="24" t="s">
+        <v>43</v>
+      </c>
+      <c r="K18" s="24">
+        <v>0</v>
+      </c>
+      <c r="L18" s="24" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="J19" t="s">
+        <v>102</v>
+      </c>
+      <c r="K19">
+        <v>2477514</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="C23" s="30" t="s">
+        <v>103</v>
+      </c>
+      <c r="D23" s="30"/>
+      <c r="E23" s="30"/>
+      <c r="F23" s="30"/>
+      <c r="G23" s="30"/>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="C24" s="19">
+        <v>32</v>
+      </c>
+      <c r="D24" s="19">
+        <v>64</v>
+      </c>
+      <c r="E24" s="19">
+        <v>128</v>
+      </c>
+      <c r="F24" s="19">
+        <v>256</v>
+      </c>
+      <c r="G24" s="19">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A25" s="31" t="s">
+        <v>0</v>
+      </c>
+      <c r="B25" s="28">
+        <v>32</v>
+      </c>
+      <c r="C25" s="1">
+        <v>0.5534</v>
+      </c>
+      <c r="D25" s="1">
+        <v>0.62729999999999897</v>
+      </c>
+      <c r="E25" s="1">
+        <v>0.66810000000000003</v>
+      </c>
+      <c r="F25" s="1">
+        <v>0.67979999999999896</v>
+      </c>
+      <c r="G25" s="1">
+        <v>0.71589999999999898</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A26" s="32"/>
+      <c r="B26" s="28">
+        <v>128</v>
+      </c>
+      <c r="C26" s="1">
+        <v>0.52180000000000004</v>
+      </c>
+      <c r="D26" s="1">
+        <v>0.64119999999999899</v>
+      </c>
+      <c r="E26" s="1">
+        <v>0.64910000000000001</v>
+      </c>
+      <c r="F26" s="1">
+        <v>0.64970000000000006</v>
+      </c>
+      <c r="G26" s="27">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A27" s="33"/>
+      <c r="B27" s="28">
+        <v>512</v>
+      </c>
+      <c r="C27" s="1">
+        <v>0.55620000000000003</v>
+      </c>
+      <c r="D27" s="1">
+        <v>0.56559999999999899</v>
+      </c>
+      <c r="E27" s="1">
+        <v>0.60070000000000001</v>
+      </c>
+      <c r="F27" s="1">
+        <v>0.61050000000000004</v>
+      </c>
+      <c r="G27" s="1">
+        <v>0.63229999999999997</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="A5:A9"/>
+    <mergeCell ref="C3:E3"/>
+    <mergeCell ref="C23:G23"/>
+    <mergeCell ref="A25:A27"/>
+  </mergeCells>
+  <conditionalFormatting sqref="C5:C9 D5:E8">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C25:G25 C26:F27">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:G10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2052,13 +3231,13 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="C4" s="19" t="s">
-        <v>0</v>
-      </c>
-      <c r="D4" s="19"/>
-      <c r="E4" s="19"/>
-      <c r="F4" s="19"/>
-      <c r="G4" s="19"/>
+      <c r="C4" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="D4" s="29"/>
+      <c r="E4" s="29"/>
+      <c r="F4" s="29"/>
+      <c r="G4" s="29"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C5" s="2">
@@ -2078,7 +3257,7 @@
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6" s="20" t="s">
+      <c r="A6" s="30" t="s">
         <v>1</v>
       </c>
       <c r="B6" s="2">
@@ -2101,7 +3280,7 @@
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A7" s="20"/>
+      <c r="A7" s="30"/>
       <c r="B7" s="2">
         <v>8</v>
       </c>
@@ -2122,7 +3301,7 @@
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A8" s="20"/>
+      <c r="A8" s="30"/>
       <c r="B8" s="2">
         <v>16</v>
       </c>
@@ -2143,7 +3322,7 @@
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A9" s="20"/>
+      <c r="A9" s="30"/>
       <c r="B9" s="2">
         <v>32</v>
       </c>
@@ -2164,7 +3343,7 @@
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A10" s="20"/>
+      <c r="A10" s="30"/>
       <c r="B10" s="2">
         <v>64</v>
       </c>

</xml_diff>

<commit_message>
Redo CNN1 mnist (confusion matrix)
</commit_message>
<xml_diff>
--- a/resultats/cnn_gridsearch.xlsx
+++ b/resultats/cnn_gridsearch.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1600" yWindow="560" windowWidth="26140" windowHeight="17560" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="2200" yWindow="440" windowWidth="26140" windowHeight="17560" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="MNIST-CNN1" sheetId="2" r:id="rId1"/>
@@ -21,10 +21,11 @@
   <definedNames>
     <definedName name="gridsearch" localSheetId="3">'CIFAR10-CNN2'!$C$5:$E$9</definedName>
     <definedName name="gridsearch" localSheetId="4">Essai!$C$6:$G$10</definedName>
+    <definedName name="gridsearch" localSheetId="0">'MNIST-CNN1'!$C$5:$E$7</definedName>
     <definedName name="gridsearch" localSheetId="2">'MNIST-CNN2'!$C$5:$E$9</definedName>
     <definedName name="gridsearch_1" localSheetId="1">'CIFAR10-CNN1'!$C$19:$H$25</definedName>
     <definedName name="gridsearch_1" localSheetId="3">'CIFAR10-CNN2'!$C$25:$E$29</definedName>
-    <definedName name="gridsearch_1" localSheetId="0">'MNIST-CNN1'!$C$5:$G$9</definedName>
+    <definedName name="gridsearch_1" localSheetId="2">'MNIST-CNN2'!$C$24:$E$28</definedName>
     <definedName name="gridsearch_2" localSheetId="1">'CIFAR10-CNN1'!$C$5:$G$10</definedName>
   </definedNames>
   <calcPr calcId="150000" concurrentCalc="0"/>
@@ -52,18 +53,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="2" name="gridsearch1" type="6" refreshedVersion="0" background="1" saveData="1">
-    <textPr fileType="mac" sourceFile="/Users/carl/Documents/uni/RecFormesAnalyseIm/Analyse_dimage_avance_proj/gridsearch.csv" thousands=" ">
-      <textFields count="5">
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-      </textFields>
-    </textPr>
-  </connection>
-  <connection id="3" name="gridsearch2" type="6" refreshedVersion="0" background="1" saveData="1">
+  <connection id="2" name="gridsearch2" type="6" refreshedVersion="0" background="1" saveData="1">
     <textPr fileType="mac" sourceFile="/Users/carl/Documents/uni/RecFormesAnalyseIm/Analyse_dimage_avance_proj/gridsearch.csv" thousands=" ">
       <textFields count="3">
         <textField/>
@@ -72,7 +62,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="4" name="gridsearch21" type="6" refreshedVersion="0" background="1" saveData="1">
+  <connection id="3" name="gridsearch21" type="6" refreshedVersion="0" background="1" saveData="1">
     <textPr fileType="mac" sourceFile="/Users/carl/Documents/uni/RecFormesAnalyseIm/Analyse_dimage_avance_proj/gridsearch.csv" thousands=" ">
       <textFields count="3">
         <textField/>
@@ -81,7 +71,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="5" name="gridsearch3" type="6" refreshedVersion="0" background="1" saveData="1">
+  <connection id="4" name="gridsearch3" type="6" refreshedVersion="0" background="1" saveData="1">
     <textPr fileType="mac" sourceFile="/Users/carl/Documents/uni/RecFormesAnalyseIm/Analyse_dimage_avance_proj/gridsearch.csv" thousands=" ">
       <textFields count="7">
         <textField/>
@@ -94,7 +84,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="6" name="gridsearch4" type="6" refreshedVersion="0" background="1" saveData="1">
+  <connection id="5" name="gridsearch4" type="6" refreshedVersion="0" background="1" saveData="1">
     <textPr fileType="mac" sourceFile="/Users/carl/Documents/uni/RecFormesAnalyseIm/Analyse_dimage_avance_proj/gridsearch.csv" thousands=" ">
       <textFields count="5">
         <textField/>
@@ -105,7 +95,25 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="7" name="gridsearch5" type="6" refreshedVersion="0" background="1" saveData="1">
+  <connection id="6" name="gridsearch5" type="6" refreshedVersion="0" background="1" saveData="1">
+    <textPr fileType="mac" sourceFile="/Users/carl/Documents/uni/RecFormesAnalyseIm/Analyse_dimage_avance_proj/gridsearch.csv" thousands=" ">
+      <textFields count="3">
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="7" name="gridsearch51" type="6" refreshedVersion="0" background="1" saveData="1">
+    <textPr fileType="mac" sourceFile="/Users/carl/Documents/uni/RecFormesAnalyseIm/Analyse_dimage_avance_proj/gridsearch.csv" thousands=" ">
+      <textFields count="3">
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="8" name="gridsearch6" type="6" refreshedVersion="0" background="1" saveData="1">
     <textPr fileType="mac" codePage="10000" sourceFile="/Users/carl/Documents/uni/RecFormesAnalyseIm/Analyse_dimage_avance_proj/gridsearch.csv" thousands=" ">
       <textFields count="3">
         <textField/>
@@ -118,7 +126,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="113">
   <si>
     <t>Batch size</t>
   </si>
@@ -463,9 +471,6 @@
     <t>Filter config</t>
   </si>
   <si>
-    <t>Refaire car persistence des poids</t>
-  </si>
-  <si>
     <t>convolution2d_13 (Convolution2D)</t>
   </si>
   <si>
@@ -608,6 +613,9 @@
   </si>
   <si>
     <t>Total params</t>
+  </si>
+  <si>
+    <t>4, 4, 8, 8</t>
   </si>
 </sst>
 </file>
@@ -672,7 +680,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -687,24 +695,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC00000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFF9696B"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -793,8 +789,50 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="63">
+  <cellStyleXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -858,17 +896,18 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="10" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="10" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -889,7 +928,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -897,10 +935,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="10" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="10" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -916,9 +959,33 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="63">
+  <cellStyles count="67">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="5" builtinId="8" hidden="1"/>
@@ -950,6 +1017,8 @@
     <cellStyle name="Lien hypertexte" xfId="57" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="59" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="65" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="6" builtinId="9" hidden="1"/>
@@ -981,6 +1050,8 @@
     <cellStyle name="Lien hypertexte visité" xfId="58" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="60" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="66" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -999,30 +1070,34 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="gridsearch_1" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="gridsearch" connectionId="8" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="gridsearch_2" connectionId="6" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="gridsearch_2" connectionId="5" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="gridsearch_1" connectionId="5" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="gridsearch_1" connectionId="4" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="gridsearch" connectionId="7" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="gridsearch_1" connectionId="7" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable5.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="gridsearch_1" connectionId="4" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="gridsearch" connectionId="6" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable6.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="gridsearch" connectionId="3" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="gridsearch_1" connectionId="3" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable7.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="gridsearch" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable8.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="gridsearch" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
@@ -1289,15 +1364,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I13"/>
+  <dimension ref="A1:L26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+      <selection activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="5.33203125" customWidth="1"/>
+    <col min="1" max="1" width="8.1640625" customWidth="1"/>
+    <col min="2" max="2" width="12.1640625" customWidth="1"/>
+    <col min="3" max="10" width="8.6640625" customWidth="1"/>
+    <col min="11" max="13" width="8.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
@@ -1306,214 +1384,128 @@
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="C3" s="29" t="s">
-        <v>0</v>
-      </c>
-      <c r="D3" s="29"/>
-      <c r="E3" s="29"/>
-      <c r="F3" s="29"/>
-      <c r="G3" s="29"/>
-      <c r="H3" s="29"/>
-      <c r="I3" s="29"/>
+      <c r="C3" s="34" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" s="35"/>
+      <c r="E3" s="35"/>
+      <c r="F3" s="43"/>
+      <c r="G3" s="17"/>
+      <c r="H3" s="17"/>
+      <c r="I3" s="17"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C4" s="2">
+        <v>16</v>
+      </c>
+      <c r="D4" s="2">
+        <v>32</v>
+      </c>
+      <c r="E4" s="42">
         <v>64</v>
       </c>
-      <c r="D4" s="2">
-        <v>128</v>
-      </c>
-      <c r="E4" s="2">
-        <v>256</v>
-      </c>
-      <c r="F4" s="2">
-        <v>512</v>
-      </c>
-      <c r="G4" s="2">
-        <v>1024</v>
-      </c>
-      <c r="H4" s="5">
-        <v>2048</v>
-      </c>
-      <c r="I4" s="5">
-        <v>4096</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A5" s="30" t="s">
+      <c r="F4" s="44"/>
+      <c r="G4" s="39"/>
+      <c r="H4" s="5"/>
+      <c r="I4" s="5"/>
+    </row>
+    <row r="5" spans="1:9" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="2">
-        <v>4</v>
+      <c r="B5" s="2" t="s">
+        <v>112</v>
       </c>
       <c r="C5" s="1">
-        <v>0.95799999999999896</v>
+        <v>0.97289999999999899</v>
       </c>
       <c r="D5" s="1">
-        <v>0.96550000000000002</v>
+        <v>0.96950000000000003</v>
       </c>
       <c r="E5" s="1">
-        <v>0.96709999999999896</v>
-      </c>
-      <c r="F5" s="1">
-        <v>0.96889999999999898</v>
-      </c>
-      <c r="G5" s="1">
-        <v>0.96960000000000002</v>
-      </c>
-      <c r="H5" s="1">
-        <v>0.90900000000000003</v>
-      </c>
-      <c r="I5" s="1">
-        <v>0.94200000000000006</v>
-      </c>
+        <v>0.96930000000000005</v>
+      </c>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A6" s="30"/>
-      <c r="B6" s="2">
-        <v>8</v>
+      <c r="A6" s="37"/>
+      <c r="B6" s="2" t="s">
+        <v>57</v>
       </c>
       <c r="C6" s="1">
-        <v>0.974799999999999</v>
+        <v>0.98429999999999895</v>
       </c>
       <c r="D6" s="1">
-        <v>0.98089999999999899</v>
+        <v>0.98340000000000005</v>
       </c>
       <c r="E6" s="1">
-        <v>0.98270000000000002</v>
-      </c>
-      <c r="F6" s="1">
-        <v>0.98529999999999895</v>
-      </c>
-      <c r="G6" s="1">
-        <v>0.98670000000000002</v>
-      </c>
-      <c r="H6" s="1">
-        <v>0.94399999999999995</v>
-      </c>
-      <c r="I6" s="1">
-        <v>0.95299999999999996</v>
-      </c>
+        <v>0.98019999999999896</v>
+      </c>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A7" s="30"/>
-      <c r="B7" s="2">
-        <v>16</v>
+      <c r="A7" s="37"/>
+      <c r="B7" s="38" t="s">
+        <v>59</v>
       </c>
       <c r="C7" s="1">
-        <v>0.98240000000000005</v>
+        <v>0.98929999999999896</v>
       </c>
       <c r="D7" s="1">
-        <v>0.98799999999999899</v>
+        <v>0.98919999999999897</v>
       </c>
       <c r="E7" s="1">
-        <v>0.99060000000000004</v>
-      </c>
-      <c r="F7" s="1">
-        <v>0.9909</v>
-      </c>
-      <c r="G7" s="1">
-        <v>0.99050000000000005</v>
-      </c>
-      <c r="H7" s="1">
-        <v>0.95199999999999996</v>
-      </c>
-      <c r="I7" s="1">
-        <v>0.96400000000000008</v>
-      </c>
+        <v>0.984899999999999</v>
+      </c>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A8" s="30"/>
-      <c r="B8" s="2">
-        <v>32</v>
-      </c>
-      <c r="C8" s="1">
-        <v>0.98970000000000002</v>
-      </c>
-      <c r="D8" s="1">
-        <v>0.99229999999999896</v>
-      </c>
-      <c r="E8" s="1">
-        <v>0.99250000000000005</v>
-      </c>
-      <c r="F8" s="1">
-        <v>0.99390000000000001</v>
-      </c>
-      <c r="G8" s="1">
-        <v>0.99409999999999898</v>
-      </c>
-      <c r="H8" s="1">
-        <v>0.95399999999999996</v>
-      </c>
-      <c r="I8" s="1">
-        <v>0.96900000000000008</v>
-      </c>
+      <c r="A8" s="40"/>
+      <c r="B8" s="41"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A9" s="30"/>
-      <c r="B9" s="2">
-        <v>64</v>
-      </c>
-      <c r="C9" s="1">
-        <v>0.99029999999999896</v>
-      </c>
-      <c r="D9" s="1">
-        <v>0.99339999999999895</v>
-      </c>
-      <c r="E9" s="1">
-        <v>0.99409999999999898</v>
-      </c>
-      <c r="F9" s="1">
-        <v>0.99450000000000005</v>
-      </c>
-      <c r="G9" s="1">
-        <v>0.99409999999999898</v>
-      </c>
-      <c r="H9" s="1">
-        <v>0.96799999999999997</v>
-      </c>
-      <c r="I9" s="4">
-        <v>0.97799999999999998</v>
-      </c>
+      <c r="A9" s="14"/>
+      <c r="B9" s="39"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="4"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A10" s="30"/>
-      <c r="B10" s="5">
-        <v>128</v>
-      </c>
-      <c r="C10" s="1">
-        <v>0.99199999999999999</v>
-      </c>
-      <c r="D10" s="1">
-        <v>0.99400000000000011</v>
-      </c>
-      <c r="E10" s="1">
-        <v>0.99400000000000011</v>
-      </c>
-      <c r="F10" s="1">
-        <v>0.995</v>
-      </c>
-      <c r="G10" s="1">
-        <v>0.995</v>
-      </c>
-      <c r="H10" s="1">
-        <v>0.995</v>
-      </c>
-      <c r="I10" s="1">
-        <v>0.995</v>
-      </c>
+      <c r="A10" s="14"/>
+      <c r="B10" s="5"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A11" s="30"/>
-      <c r="B11" s="5">
-        <v>256</v>
-      </c>
-      <c r="C11" s="8">
-        <v>0.114</v>
-      </c>
-      <c r="D11" s="8">
-        <v>0.114</v>
-      </c>
+      <c r="A11" s="14"/>
+      <c r="B11" s="5"/>
+      <c r="C11" s="6"/>
+      <c r="D11" s="6"/>
       <c r="E11" s="7"/>
       <c r="F11" s="7"/>
       <c r="G11" s="7"/>
@@ -1521,26 +1513,144 @@
       <c r="I11" s="7"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B12" s="6"/>
+      <c r="B12" s="5"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A13" s="21" t="s">
-        <v>64</v>
-      </c>
-      <c r="B13" s="21"/>
-      <c r="C13" s="21"/>
-      <c r="D13" s="21"/>
-      <c r="E13" s="21"/>
-      <c r="F13" s="21"/>
-      <c r="G13" s="21"/>
+      <c r="A13" s="33"/>
+      <c r="B13" s="33"/>
+      <c r="C13" s="33"/>
+      <c r="D13" s="33"/>
+      <c r="E13" s="33"/>
+      <c r="F13" s="33"/>
+      <c r="G13" s="33"/>
+    </row>
+    <row r="17" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="C17" s="27"/>
+      <c r="D17" s="27"/>
+      <c r="E17" s="27"/>
+      <c r="F17" s="27"/>
+      <c r="G17" s="27"/>
+      <c r="H17" s="27"/>
+      <c r="I17" s="27"/>
+      <c r="J17" s="27"/>
+      <c r="K17" s="27"/>
+      <c r="L17" s="27"/>
+    </row>
+    <row r="18" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="C18" s="27"/>
+      <c r="D18" s="27"/>
+      <c r="E18" s="27"/>
+      <c r="F18" s="27"/>
+      <c r="G18" s="27"/>
+      <c r="H18" s="27"/>
+      <c r="I18" s="27"/>
+      <c r="J18" s="27"/>
+      <c r="K18" s="27"/>
+      <c r="L18" s="27"/>
+    </row>
+    <row r="19" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="C19" s="27"/>
+      <c r="D19" s="27"/>
+      <c r="E19" s="27"/>
+      <c r="F19" s="27"/>
+      <c r="G19" s="27"/>
+      <c r="H19" s="27"/>
+      <c r="I19" s="27"/>
+      <c r="J19" s="27"/>
+      <c r="K19" s="27"/>
+      <c r="L19" s="27"/>
+    </row>
+    <row r="20" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="C20" s="27"/>
+      <c r="D20" s="27"/>
+      <c r="E20" s="27"/>
+      <c r="F20" s="27"/>
+      <c r="G20" s="27"/>
+      <c r="H20" s="27"/>
+      <c r="I20" s="27"/>
+      <c r="J20" s="27"/>
+      <c r="K20" s="27"/>
+      <c r="L20" s="27"/>
+    </row>
+    <row r="21" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="C21" s="27"/>
+      <c r="D21" s="27"/>
+      <c r="E21" s="27"/>
+      <c r="F21" s="27"/>
+      <c r="G21" s="27"/>
+      <c r="H21" s="27"/>
+      <c r="I21" s="27"/>
+      <c r="J21" s="27"/>
+      <c r="K21" s="27"/>
+      <c r="L21" s="27"/>
+    </row>
+    <row r="22" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="C22" s="27"/>
+      <c r="D22" s="27"/>
+      <c r="E22" s="27"/>
+      <c r="F22" s="27"/>
+      <c r="G22" s="27"/>
+      <c r="H22" s="27"/>
+      <c r="I22" s="27"/>
+      <c r="J22" s="27"/>
+      <c r="K22" s="27"/>
+      <c r="L22" s="27"/>
+    </row>
+    <row r="23" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="C23" s="27"/>
+      <c r="D23" s="27"/>
+      <c r="E23" s="27"/>
+      <c r="F23" s="27"/>
+      <c r="G23" s="27"/>
+      <c r="H23" s="27"/>
+      <c r="I23" s="27"/>
+      <c r="J23" s="27"/>
+      <c r="K23" s="27"/>
+      <c r="L23" s="27"/>
+    </row>
+    <row r="24" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="C24" s="27"/>
+      <c r="D24" s="27"/>
+      <c r="E24" s="27"/>
+      <c r="F24" s="27"/>
+      <c r="G24" s="27"/>
+      <c r="H24" s="27"/>
+      <c r="I24" s="27"/>
+      <c r="J24" s="27"/>
+      <c r="K24" s="27"/>
+      <c r="L24" s="27"/>
+    </row>
+    <row r="25" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="C25" s="27"/>
+      <c r="D25" s="27"/>
+      <c r="E25" s="27"/>
+      <c r="F25" s="27"/>
+      <c r="G25" s="27"/>
+      <c r="H25" s="27"/>
+      <c r="I25" s="27"/>
+      <c r="J25" s="27"/>
+      <c r="K25" s="27"/>
+      <c r="L25" s="27"/>
+    </row>
+    <row r="26" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="C26" s="27"/>
+      <c r="D26" s="27"/>
+      <c r="E26" s="27"/>
+      <c r="F26" s="27"/>
+      <c r="G26" s="27"/>
+      <c r="H26" s="27"/>
+      <c r="I26" s="27"/>
+      <c r="J26" s="27"/>
+      <c r="K26" s="27"/>
+      <c r="L26" s="27"/>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="C3:I3"/>
-    <mergeCell ref="A5:A11"/>
+    <mergeCell ref="C3:E3"/>
+    <mergeCell ref="A5:A7"/>
   </mergeCells>
-  <conditionalFormatting sqref="C5:G9 C11:I11">
-    <cfRule type="colorScale" priority="3">
+  <conditionalFormatting sqref="C8:G9 C11:I11 F5:G7">
+    <cfRule type="colorScale" priority="6">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -1551,7 +1661,31 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C7:G9 C11:I11">
+  <conditionalFormatting sqref="C8:G9 C11:I11 F7:G7">
+    <cfRule type="colorScale" priority="7">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C8:I12 F5:I7">
+    <cfRule type="colorScale" priority="5">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C8:I10 F5:I7">
     <cfRule type="colorScale" priority="4">
       <colorScale>
         <cfvo type="min"/>
@@ -1563,19 +1697,27 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C5:I12">
+  <conditionalFormatting sqref="C17:L26">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
         <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFCFCFF"/>
         <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
         <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
+        <color rgb="FFF8696B"/>
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C5:I10">
+  <conditionalFormatting sqref="C5:E7">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
@@ -1618,35 +1760,35 @@
       </c>
     </row>
     <row r="2" spans="1:16" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="I2" s="16" t="s">
+      <c r="I2" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="J2" s="16"/>
-      <c r="K2" s="16"/>
-      <c r="L2" s="16"/>
-      <c r="M2" s="12"/>
-      <c r="N2" s="12"/>
-      <c r="O2" s="12"/>
+      <c r="J2" s="13"/>
+      <c r="K2" s="13"/>
+      <c r="L2" s="13"/>
+      <c r="M2" s="9"/>
+      <c r="N2" s="9"/>
+      <c r="O2" s="9"/>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="C3" s="29" t="s">
-        <v>0</v>
-      </c>
-      <c r="D3" s="29"/>
-      <c r="E3" s="29"/>
-      <c r="F3" s="29"/>
-      <c r="G3" s="29"/>
-      <c r="H3" s="20"/>
-      <c r="I3" s="13" t="s">
+      <c r="C3" s="28" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" s="28"/>
+      <c r="E3" s="28"/>
+      <c r="F3" s="28"/>
+      <c r="G3" s="28"/>
+      <c r="H3" s="17"/>
+      <c r="I3" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="J3" s="13" t="s">
+      <c r="J3" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="K3" s="13" t="s">
+      <c r="K3" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="L3" s="13" t="s">
+      <c r="L3" s="10" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1666,22 +1808,22 @@
       <c r="G4" s="2">
         <v>128</v>
       </c>
-      <c r="H4" s="6"/>
-      <c r="I4" s="12" t="s">
+      <c r="H4" s="5"/>
+      <c r="I4" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="J4" s="12" t="s">
+      <c r="J4" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="K4" s="12">
+      <c r="K4" s="9">
         <v>448</v>
       </c>
-      <c r="L4" s="12" t="s">
+      <c r="L4" s="9" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:16" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="30" t="s">
+      <c r="A5" s="29" t="s">
         <v>63</v>
       </c>
       <c r="B5" s="2" t="s">
@@ -1703,21 +1845,21 @@
         <v>0.502</v>
       </c>
       <c r="H5" s="1"/>
-      <c r="I5" s="14" t="s">
+      <c r="I5" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="J5" s="14" t="s">
+      <c r="J5" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="K5" s="14">
-        <v>0</v>
-      </c>
-      <c r="L5" s="14" t="s">
+      <c r="K5" s="11">
+        <v>0</v>
+      </c>
+      <c r="L5" s="11" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A6" s="30"/>
+      <c r="A6" s="29"/>
       <c r="B6" s="2" t="s">
         <v>57</v>
       </c>
@@ -1737,22 +1879,22 @@
         <v>0.50839999999999896</v>
       </c>
       <c r="H6" s="1"/>
-      <c r="I6" s="12" t="s">
+      <c r="I6" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="J6" s="12" t="s">
+      <c r="J6" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="K6" s="12">
+      <c r="K6" s="9">
         <v>4640</v>
       </c>
-      <c r="L6" s="12" t="s">
+      <c r="L6" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="P6" s="11"/>
+      <c r="P6" s="8"/>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A7" s="30"/>
+      <c r="A7" s="29"/>
       <c r="B7" s="2" t="s">
         <v>58</v>
       </c>
@@ -1772,22 +1914,22 @@
         <v>0.5776</v>
       </c>
       <c r="H7" s="1"/>
-      <c r="I7" s="12" t="s">
+      <c r="I7" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="J7" s="12" t="s">
+      <c r="J7" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="K7" s="12">
-        <v>0</v>
-      </c>
-      <c r="L7" s="12" t="s">
+      <c r="K7" s="9">
+        <v>0</v>
+      </c>
+      <c r="L7" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="P7" s="11"/>
+      <c r="P7" s="8"/>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A8" s="30"/>
+      <c r="A8" s="29"/>
       <c r="B8" s="2" t="s">
         <v>59</v>
       </c>
@@ -1807,22 +1949,22 @@
         <v>0.56889999999999896</v>
       </c>
       <c r="H8" s="1"/>
-      <c r="I8" s="12" t="s">
+      <c r="I8" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="J8" s="12" t="s">
+      <c r="J8" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="K8" s="12">
-        <v>0</v>
-      </c>
-      <c r="L8" s="12" t="s">
+      <c r="K8" s="9">
+        <v>0</v>
+      </c>
+      <c r="L8" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="P8" s="11"/>
+      <c r="P8" s="8"/>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A9" s="30"/>
+      <c r="A9" s="29"/>
       <c r="B9" s="2" t="s">
         <v>60</v>
       </c>
@@ -1841,23 +1983,23 @@
       <c r="G9" s="1">
         <v>0.61750000000000005</v>
       </c>
-      <c r="H9" s="10"/>
-      <c r="I9" s="14" t="s">
+      <c r="H9" s="7"/>
+      <c r="I9" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="J9" s="14" t="s">
+      <c r="J9" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="K9" s="14">
-        <v>0</v>
-      </c>
-      <c r="L9" s="14" t="s">
+      <c r="K9" s="11">
+        <v>0</v>
+      </c>
+      <c r="L9" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="P9" s="11"/>
+      <c r="P9" s="8"/>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A10" s="30"/>
+      <c r="A10" s="29"/>
       <c r="B10" s="2" t="s">
         <v>61</v>
       </c>
@@ -1877,218 +2019,218 @@
         <v>0.61180000000000001</v>
       </c>
       <c r="H10" s="1"/>
-      <c r="I10" s="12" t="s">
+      <c r="I10" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="J10" s="12" t="s">
+      <c r="J10" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="K10" s="12">
+      <c r="K10" s="9">
         <v>18496</v>
       </c>
-      <c r="L10" s="12" t="s">
+      <c r="L10" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="P10" s="11"/>
+      <c r="P10" s="8"/>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A11" s="17"/>
-      <c r="B11" s="6"/>
-      <c r="C11" s="9"/>
-      <c r="D11" s="9"/>
-      <c r="E11" s="10"/>
-      <c r="F11" s="10"/>
-      <c r="G11" s="10"/>
-      <c r="H11" s="10"/>
-      <c r="I11" s="14" t="s">
+      <c r="A11" s="14"/>
+      <c r="B11" s="5"/>
+      <c r="C11" s="6"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="7"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="7"/>
+      <c r="H11" s="7"/>
+      <c r="I11" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="J11" s="14" t="s">
+      <c r="J11" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="K11" s="14">
-        <v>0</v>
-      </c>
-      <c r="L11" s="14" t="s">
+      <c r="K11" s="11">
+        <v>0</v>
+      </c>
+      <c r="L11" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="P11" s="11"/>
+      <c r="P11" s="8"/>
     </row>
     <row r="12" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="I12" s="12" t="s">
+      <c r="I12" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="J12" s="12" t="s">
+      <c r="J12" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="K12" s="12">
+      <c r="K12" s="9">
         <v>73856</v>
       </c>
-      <c r="L12" s="12" t="s">
+      <c r="L12" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="P12" s="11"/>
+      <c r="P12" s="8"/>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="I13" s="12" t="s">
+      <c r="I13" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="J13" s="12" t="s">
+      <c r="J13" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="K13" s="12">
-        <v>0</v>
-      </c>
-      <c r="L13" s="12" t="s">
+      <c r="K13" s="9">
+        <v>0</v>
+      </c>
+      <c r="L13" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="P13" s="11"/>
+      <c r="P13" s="8"/>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="I14" s="15" t="s">
+      <c r="I14" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="J14" s="15" t="s">
+      <c r="J14" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="K14" s="15">
-        <v>0</v>
-      </c>
-      <c r="L14" s="15" t="s">
+      <c r="K14" s="12">
+        <v>0</v>
+      </c>
+      <c r="L14" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="P14" s="11"/>
+      <c r="P14" s="8"/>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="B15" s="12"/>
-      <c r="I15" s="15" t="s">
+      <c r="B15" s="9"/>
+      <c r="I15" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="J15" s="15" t="s">
+      <c r="J15" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="K15" s="15">
-        <v>0</v>
-      </c>
-      <c r="L15" s="15" t="s">
+      <c r="K15" s="12">
+        <v>0</v>
+      </c>
+      <c r="L15" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="P15" s="11"/>
+      <c r="P15" s="8"/>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="B16" s="12"/>
-      <c r="I16" s="14" t="s">
+      <c r="B16" s="9"/>
+      <c r="I16" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="J16" s="14" t="s">
+      <c r="J16" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="K16" s="14">
-        <v>0</v>
-      </c>
-      <c r="L16" s="14" t="s">
+      <c r="K16" s="11">
+        <v>0</v>
+      </c>
+      <c r="L16" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="P16" s="11"/>
+      <c r="P16" s="8"/>
     </row>
     <row r="17" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B17" s="12"/>
-      <c r="I17" s="12" t="s">
+      <c r="B17" s="9"/>
+      <c r="I17" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="J17" s="12" t="s">
+      <c r="J17" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="K17" s="12">
+      <c r="K17" s="9">
         <v>409728</v>
       </c>
-      <c r="L17" s="12" t="s">
+      <c r="L17" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="P17" s="11"/>
+      <c r="P17" s="8"/>
     </row>
     <row r="18" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B18" s="12"/>
-      <c r="I18" s="12" t="s">
+      <c r="B18" s="9"/>
+      <c r="I18" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="J18" s="12" t="s">
+      <c r="J18" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="K18" s="12">
-        <v>0</v>
-      </c>
-      <c r="L18" s="12" t="s">
+      <c r="K18" s="9">
+        <v>0</v>
+      </c>
+      <c r="L18" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="P18" s="11"/>
+      <c r="P18" s="8"/>
     </row>
     <row r="19" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B19" s="12"/>
-      <c r="I19" s="14" t="s">
+      <c r="B19" s="9"/>
+      <c r="I19" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="J19" s="14" t="s">
+      <c r="J19" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="K19" s="14">
-        <v>0</v>
-      </c>
-      <c r="L19" s="14" t="s">
+      <c r="K19" s="11">
+        <v>0</v>
+      </c>
+      <c r="L19" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="P19" s="11"/>
+      <c r="P19" s="8"/>
     </row>
     <row r="20" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B20" s="12"/>
-      <c r="I20" s="12" t="s">
+      <c r="B20" s="9"/>
+      <c r="I20" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="J20" s="12" t="s">
+      <c r="J20" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="K20" s="12">
+      <c r="K20" s="9">
         <v>1290</v>
       </c>
-      <c r="L20" s="12" t="s">
+      <c r="L20" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="P20" s="11"/>
+      <c r="P20" s="8"/>
     </row>
     <row r="21" spans="2:16" x14ac:dyDescent="0.2">
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
       <c r="G21" s="1"/>
-      <c r="I21" s="12" t="s">
+      <c r="I21" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="J21" s="12" t="s">
+      <c r="J21" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="K21" s="12">
-        <v>0</v>
-      </c>
-      <c r="L21" s="12" t="s">
+      <c r="K21" s="9">
+        <v>0</v>
+      </c>
+      <c r="L21" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="P21" s="11"/>
+      <c r="P21" s="8"/>
     </row>
     <row r="22" spans="2:16" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="I22" s="13"/>
-      <c r="J22" s="18" t="s">
+      <c r="I22" s="10"/>
+      <c r="J22" s="15" t="s">
         <v>55</v>
       </c>
-      <c r="K22" s="13">
+      <c r="K22" s="10">
         <v>508458</v>
       </c>
-      <c r="L22" s="13"/>
-      <c r="P22" s="11"/>
+      <c r="L22" s="10"/>
+      <c r="P22" s="8"/>
     </row>
     <row r="23" spans="2:16" x14ac:dyDescent="0.2">
       <c r="G23" s="1"/>
       <c r="H23" s="1"/>
-      <c r="P23" s="11"/>
+      <c r="P23" s="8"/>
     </row>
     <row r="24" spans="2:16" x14ac:dyDescent="0.2">
       <c r="C24" s="1"/>
@@ -2097,7 +2239,7 @@
       <c r="F24" s="1"/>
       <c r="G24" s="1"/>
       <c r="H24" s="1"/>
-      <c r="P24" s="11"/>
+      <c r="P24" s="8"/>
     </row>
     <row r="25" spans="2:16" x14ac:dyDescent="0.2">
       <c r="C25" s="1"/>
@@ -2106,205 +2248,205 @@
       <c r="F25" s="1"/>
       <c r="G25" s="1"/>
       <c r="H25" s="1"/>
-      <c r="P25" s="11"/>
+      <c r="P25" s="8"/>
     </row>
     <row r="26" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="P26" s="11"/>
+      <c r="P26" s="8"/>
     </row>
     <row r="27" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="P27" s="11"/>
+      <c r="P27" s="8"/>
     </row>
     <row r="28" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="P28" s="11"/>
+      <c r="P28" s="8"/>
     </row>
     <row r="29" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="P29" s="11"/>
+      <c r="P29" s="8"/>
     </row>
     <row r="30" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="P30" s="11"/>
+      <c r="P30" s="8"/>
     </row>
     <row r="32" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="M32" s="12"/>
-      <c r="N32" s="12"/>
-      <c r="O32" s="12"/>
-      <c r="P32" s="11"/>
+      <c r="M32" s="9"/>
+      <c r="N32" s="9"/>
+      <c r="O32" s="9"/>
+      <c r="P32" s="8"/>
     </row>
     <row r="33" spans="3:16" x14ac:dyDescent="0.2">
-      <c r="P33" s="11"/>
+      <c r="P33" s="8"/>
     </row>
     <row r="34" spans="3:16" x14ac:dyDescent="0.2">
-      <c r="M34" s="12"/>
-      <c r="N34" s="12"/>
-      <c r="O34" s="12"/>
-      <c r="P34" s="11"/>
+      <c r="M34" s="9"/>
+      <c r="N34" s="9"/>
+      <c r="O34" s="9"/>
+      <c r="P34" s="8"/>
     </row>
     <row r="35" spans="3:16" x14ac:dyDescent="0.2">
-      <c r="M35" s="12"/>
-      <c r="N35" s="12"/>
-      <c r="O35" s="12"/>
+      <c r="M35" s="9"/>
+      <c r="N35" s="9"/>
+      <c r="O35" s="9"/>
     </row>
     <row r="36" spans="3:16" x14ac:dyDescent="0.2">
-      <c r="M36" s="12"/>
-      <c r="N36" s="12"/>
-      <c r="O36" s="12"/>
+      <c r="M36" s="9"/>
+      <c r="N36" s="9"/>
+      <c r="O36" s="9"/>
     </row>
     <row r="37" spans="3:16" x14ac:dyDescent="0.2">
-      <c r="M37" s="12"/>
-      <c r="N37" s="12"/>
-      <c r="O37" s="12"/>
+      <c r="M37" s="9"/>
+      <c r="N37" s="9"/>
+      <c r="O37" s="9"/>
     </row>
     <row r="38" spans="3:16" x14ac:dyDescent="0.2">
-      <c r="M38" s="12"/>
-      <c r="N38" s="12"/>
-      <c r="O38" s="12"/>
+      <c r="M38" s="9"/>
+      <c r="N38" s="9"/>
+      <c r="O38" s="9"/>
     </row>
     <row r="39" spans="3:16" x14ac:dyDescent="0.2">
-      <c r="M39" s="12"/>
-      <c r="N39" s="12"/>
-      <c r="O39" s="12"/>
+      <c r="M39" s="9"/>
+      <c r="N39" s="9"/>
+      <c r="O39" s="9"/>
     </row>
     <row r="40" spans="3:16" x14ac:dyDescent="0.2">
-      <c r="M40" s="12"/>
-      <c r="N40" s="12"/>
-      <c r="O40" s="12"/>
+      <c r="M40" s="9"/>
+      <c r="N40" s="9"/>
+      <c r="O40" s="9"/>
     </row>
     <row r="41" spans="3:16" x14ac:dyDescent="0.2">
-      <c r="M41" s="12"/>
-      <c r="N41" s="12"/>
-      <c r="O41" s="12"/>
+      <c r="M41" s="9"/>
+      <c r="N41" s="9"/>
+      <c r="O41" s="9"/>
     </row>
     <row r="42" spans="3:16" x14ac:dyDescent="0.2">
-      <c r="M42" s="12"/>
-      <c r="N42" s="12"/>
-      <c r="O42" s="12"/>
+      <c r="M42" s="9"/>
+      <c r="N42" s="9"/>
+      <c r="O42" s="9"/>
     </row>
     <row r="43" spans="3:16" x14ac:dyDescent="0.2">
-      <c r="M43" s="12"/>
-      <c r="N43" s="12"/>
-      <c r="O43" s="12"/>
+      <c r="M43" s="9"/>
+      <c r="N43" s="9"/>
+      <c r="O43" s="9"/>
     </row>
     <row r="44" spans="3:16" x14ac:dyDescent="0.2">
-      <c r="M44" s="12"/>
-      <c r="N44" s="12"/>
-      <c r="O44" s="12"/>
+      <c r="M44" s="9"/>
+      <c r="N44" s="9"/>
+      <c r="O44" s="9"/>
     </row>
     <row r="45" spans="3:16" x14ac:dyDescent="0.2">
-      <c r="C45" s="12"/>
-      <c r="D45" s="12"/>
-      <c r="M45" s="12"/>
-      <c r="N45" s="12"/>
-      <c r="O45" s="12"/>
+      <c r="C45" s="9"/>
+      <c r="D45" s="9"/>
+      <c r="M45" s="9"/>
+      <c r="N45" s="9"/>
+      <c r="O45" s="9"/>
     </row>
     <row r="46" spans="3:16" x14ac:dyDescent="0.2">
-      <c r="C46" s="12"/>
-      <c r="D46" s="12"/>
-      <c r="M46" s="12"/>
-      <c r="N46" s="12"/>
-      <c r="O46" s="12"/>
+      <c r="C46" s="9"/>
+      <c r="D46" s="9"/>
+      <c r="M46" s="9"/>
+      <c r="N46" s="9"/>
+      <c r="O46" s="9"/>
     </row>
     <row r="47" spans="3:16" x14ac:dyDescent="0.2">
-      <c r="C47" s="12"/>
-      <c r="D47" s="12"/>
-      <c r="M47" s="12"/>
-      <c r="N47" s="12"/>
-      <c r="O47" s="12"/>
+      <c r="C47" s="9"/>
+      <c r="D47" s="9"/>
+      <c r="M47" s="9"/>
+      <c r="N47" s="9"/>
+      <c r="O47" s="9"/>
     </row>
     <row r="48" spans="3:16" x14ac:dyDescent="0.2">
-      <c r="C48" s="12"/>
-      <c r="D48" s="12"/>
-      <c r="M48" s="12"/>
-      <c r="N48" s="12"/>
-      <c r="O48" s="12"/>
+      <c r="C48" s="9"/>
+      <c r="D48" s="9"/>
+      <c r="M48" s="9"/>
+      <c r="N48" s="9"/>
+      <c r="O48" s="9"/>
     </row>
     <row r="49" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="C49" s="12"/>
-      <c r="D49" s="12"/>
-      <c r="M49" s="12"/>
-      <c r="N49" s="12"/>
-      <c r="O49" s="12"/>
+      <c r="C49" s="9"/>
+      <c r="D49" s="9"/>
+      <c r="M49" s="9"/>
+      <c r="N49" s="9"/>
+      <c r="O49" s="9"/>
     </row>
     <row r="50" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="C50" s="12"/>
-      <c r="D50" s="12"/>
-      <c r="M50" s="12"/>
-      <c r="N50" s="12"/>
-      <c r="O50" s="12"/>
+      <c r="C50" s="9"/>
+      <c r="D50" s="9"/>
+      <c r="M50" s="9"/>
+      <c r="N50" s="9"/>
+      <c r="O50" s="9"/>
     </row>
     <row r="51" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B51" s="11"/>
-      <c r="C51" s="12"/>
-      <c r="D51" s="12"/>
-      <c r="E51" s="11"/>
-      <c r="F51" s="11"/>
-      <c r="G51" s="11"/>
-      <c r="H51" s="11"/>
-      <c r="M51" s="12"/>
-      <c r="N51" s="12"/>
-      <c r="O51" s="12"/>
+      <c r="B51" s="8"/>
+      <c r="C51" s="9"/>
+      <c r="D51" s="9"/>
+      <c r="E51" s="8"/>
+      <c r="F51" s="8"/>
+      <c r="G51" s="8"/>
+      <c r="H51" s="8"/>
+      <c r="M51" s="9"/>
+      <c r="N51" s="9"/>
+      <c r="O51" s="9"/>
     </row>
     <row r="52" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B52" s="11"/>
-      <c r="C52" s="12"/>
-      <c r="D52" s="12"/>
-      <c r="E52" s="11"/>
-      <c r="F52" s="11"/>
-      <c r="G52" s="11"/>
-      <c r="H52" s="11"/>
-      <c r="M52" s="12"/>
-      <c r="N52" s="12"/>
-      <c r="O52" s="12"/>
+      <c r="B52" s="8"/>
+      <c r="C52" s="9"/>
+      <c r="D52" s="9"/>
+      <c r="E52" s="8"/>
+      <c r="F52" s="8"/>
+      <c r="G52" s="8"/>
+      <c r="H52" s="8"/>
+      <c r="M52" s="9"/>
+      <c r="N52" s="9"/>
+      <c r="O52" s="9"/>
     </row>
     <row r="53" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B53" s="11"/>
-      <c r="C53" s="12"/>
-      <c r="D53" s="12"/>
-      <c r="E53" s="11"/>
-      <c r="F53" s="11"/>
-      <c r="G53" s="11"/>
-      <c r="H53" s="11"/>
-      <c r="M53" s="12"/>
-      <c r="N53" s="12"/>
-      <c r="O53" s="12"/>
+      <c r="B53" s="8"/>
+      <c r="C53" s="9"/>
+      <c r="D53" s="9"/>
+      <c r="E53" s="8"/>
+      <c r="F53" s="8"/>
+      <c r="G53" s="8"/>
+      <c r="H53" s="8"/>
+      <c r="M53" s="9"/>
+      <c r="N53" s="9"/>
+      <c r="O53" s="9"/>
     </row>
     <row r="54" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="C54" s="12"/>
-      <c r="D54" s="12"/>
+      <c r="C54" s="9"/>
+      <c r="D54" s="9"/>
     </row>
     <row r="55" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="C55" s="12"/>
-      <c r="D55" s="12"/>
+      <c r="C55" s="9"/>
+      <c r="D55" s="9"/>
     </row>
     <row r="56" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="C56" s="12"/>
-      <c r="D56" s="12"/>
+      <c r="C56" s="9"/>
+      <c r="D56" s="9"/>
     </row>
     <row r="57" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="C57" s="12"/>
-      <c r="D57" s="12"/>
+      <c r="C57" s="9"/>
+      <c r="D57" s="9"/>
     </row>
     <row r="58" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="C58" s="12"/>
-      <c r="D58" s="12"/>
+      <c r="C58" s="9"/>
+      <c r="D58" s="9"/>
     </row>
     <row r="59" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="C59" s="12"/>
-      <c r="D59" s="12"/>
+      <c r="C59" s="9"/>
+      <c r="D59" s="9"/>
     </row>
     <row r="60" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="C60" s="12"/>
-      <c r="D60" s="12"/>
+      <c r="C60" s="9"/>
+      <c r="D60" s="9"/>
     </row>
     <row r="61" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="C61" s="12"/>
+      <c r="C61" s="9"/>
     </row>
     <row r="62" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="C62" s="12"/>
+      <c r="C62" s="9"/>
     </row>
     <row r="63" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="C63" s="12"/>
+      <c r="C63" s="9"/>
     </row>
     <row r="64" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="C64" s="12"/>
+      <c r="C64" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -2389,86 +2531,90 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J18"/>
+  <dimension ref="A1:K26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
+      <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="5.6640625" customWidth="1"/>
     <col min="3" max="5" width="8.1640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="31.33203125" customWidth="1"/>
-    <col min="8" max="8" width="18.5" customWidth="1"/>
-    <col min="9" max="9" width="8.83203125" customWidth="1"/>
-    <col min="10" max="10" width="26.33203125" customWidth="1"/>
+    <col min="6" max="6" width="8.1640625" customWidth="1"/>
+    <col min="7" max="7" width="8" customWidth="1"/>
+    <col min="8" max="8" width="31.33203125" customWidth="1"/>
+    <col min="9" max="9" width="18.5" customWidth="1"/>
+    <col min="10" max="10" width="8.83203125" customWidth="1"/>
+    <col min="11" max="11" width="26.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="G2" s="34" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="H2" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="H2" s="34" t="s">
+      <c r="I2" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="I2" s="34" t="s">
+      <c r="J2" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="J2" s="34" t="s">
+      <c r="K2" s="25" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="17" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="C3" s="29" t="s">
-        <v>0</v>
-      </c>
-      <c r="D3" s="29"/>
-      <c r="E3" s="29"/>
-      <c r="G3" t="s">
-        <v>65</v>
-      </c>
+    <row r="3" spans="1:11" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="C3" s="28" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" s="28"/>
+      <c r="E3" s="28"/>
+      <c r="F3" s="45"/>
       <c r="H3" t="s">
-        <v>107</v>
-      </c>
-      <c r="I3">
+        <v>64</v>
+      </c>
+      <c r="I3" t="s">
+        <v>106</v>
+      </c>
+      <c r="J3">
         <v>640</v>
       </c>
-      <c r="J3" t="s">
+      <c r="K3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="C4" s="18">
+        <v>32</v>
+      </c>
+      <c r="D4" s="18">
+        <v>128</v>
+      </c>
+      <c r="E4" s="18">
+        <v>512</v>
+      </c>
+      <c r="F4" s="45"/>
+      <c r="H4" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="C4" s="22">
-        <v>32</v>
-      </c>
-      <c r="D4" s="22">
-        <v>128</v>
-      </c>
-      <c r="E4" s="22">
-        <v>512</v>
-      </c>
-      <c r="G4" t="s">
+      <c r="I4" t="s">
+        <v>106</v>
+      </c>
+      <c r="J4">
+        <v>0</v>
+      </c>
+      <c r="K4" t="s">
         <v>68</v>
       </c>
-      <c r="H4" t="s">
-        <v>107</v>
-      </c>
-      <c r="I4">
-        <v>0</v>
-      </c>
-      <c r="J4" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A5" s="30" t="s">
-        <v>103</v>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A5" s="29" t="s">
+        <v>102</v>
       </c>
       <c r="B5" s="2">
         <v>32</v>
@@ -2482,21 +2628,22 @@
       <c r="E5" s="1">
         <v>0.98780000000000001</v>
       </c>
-      <c r="G5" s="25" t="s">
+      <c r="F5" s="1"/>
+      <c r="H5" s="21" t="s">
+        <v>69</v>
+      </c>
+      <c r="I5" s="21" t="s">
+        <v>106</v>
+      </c>
+      <c r="J5" s="21">
+        <v>0</v>
+      </c>
+      <c r="K5" s="21" t="s">
         <v>70</v>
       </c>
-      <c r="H5" s="25" t="s">
-        <v>107</v>
-      </c>
-      <c r="I5" s="25">
-        <v>0</v>
-      </c>
-      <c r="J5" s="25" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A6" s="30"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A6" s="29"/>
       <c r="B6" s="2">
         <v>64</v>
       </c>
@@ -2509,21 +2656,22 @@
       <c r="E6" s="1">
         <v>0.99180000000000001</v>
       </c>
-      <c r="G6" t="s">
-        <v>72</v>
-      </c>
+      <c r="F6" s="1"/>
       <c r="H6" t="s">
-        <v>108</v>
-      </c>
-      <c r="I6">
+        <v>71</v>
+      </c>
+      <c r="I6" t="s">
+        <v>107</v>
+      </c>
+      <c r="J6">
         <v>36928</v>
       </c>
-      <c r="J6" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A7" s="30"/>
+      <c r="K6" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A7" s="29"/>
       <c r="B7" s="2">
         <v>128</v>
       </c>
@@ -2536,21 +2684,22 @@
       <c r="E7" s="1">
         <v>0.99229999999999896</v>
       </c>
-      <c r="G7" t="s">
+      <c r="F7" s="1"/>
+      <c r="H7" t="s">
+        <v>74</v>
+      </c>
+      <c r="I7" t="s">
+        <v>107</v>
+      </c>
+      <c r="J7">
+        <v>0</v>
+      </c>
+      <c r="K7" t="s">
         <v>75</v>
       </c>
-      <c r="H7" t="s">
-        <v>108</v>
-      </c>
-      <c r="I7">
-        <v>0</v>
-      </c>
-      <c r="J7" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A8" s="30"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A8" s="29"/>
       <c r="B8" s="2">
         <v>256</v>
       </c>
@@ -2563,21 +2712,22 @@
       <c r="E8" s="1">
         <v>0.99239999999999895</v>
       </c>
-      <c r="G8" s="25" t="s">
-        <v>77</v>
-      </c>
-      <c r="H8" s="25" t="s">
-        <v>109</v>
-      </c>
-      <c r="I8" s="25">
-        <v>0</v>
-      </c>
-      <c r="J8" s="25" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A9" s="30"/>
+      <c r="F8" s="1"/>
+      <c r="H8" s="21" t="s">
+        <v>76</v>
+      </c>
+      <c r="I8" s="21" t="s">
+        <v>108</v>
+      </c>
+      <c r="J8" s="21">
+        <v>0</v>
+      </c>
+      <c r="K8" s="21" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A9" s="29"/>
       <c r="B9" s="2">
         <v>512</v>
       </c>
@@ -2590,145 +2740,251 @@
       <c r="E9" s="1">
         <v>0.99390000000000001</v>
       </c>
-      <c r="G9" t="s">
-        <v>80</v>
-      </c>
+      <c r="F9" s="1"/>
       <c r="H9" t="s">
+        <v>79</v>
+      </c>
+      <c r="I9" t="s">
+        <v>109</v>
+      </c>
+      <c r="J9">
+        <v>73856</v>
+      </c>
+      <c r="K9" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="H10" t="s">
+        <v>82</v>
+      </c>
+      <c r="I10" t="s">
+        <v>109</v>
+      </c>
+      <c r="J10">
+        <v>0</v>
+      </c>
+      <c r="K10" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="H11" t="s">
+        <v>84</v>
+      </c>
+      <c r="I11" t="s">
         <v>110</v>
       </c>
-      <c r="I9">
-        <v>73856</v>
-      </c>
-      <c r="J9" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="G10" t="s">
-        <v>83</v>
-      </c>
-      <c r="H10" t="s">
-        <v>110</v>
-      </c>
-      <c r="I10">
-        <v>0</v>
-      </c>
-      <c r="J10" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="G11" t="s">
-        <v>85</v>
-      </c>
-      <c r="H11" t="s">
+      <c r="J11">
+        <v>0</v>
+      </c>
+      <c r="K11" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="H12" s="21" t="s">
+        <v>87</v>
+      </c>
+      <c r="I12" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="J12" s="21">
+        <v>0</v>
+      </c>
+      <c r="K12" s="21" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="H13" t="s">
+        <v>90</v>
+      </c>
+      <c r="I13" t="s">
+        <v>91</v>
+      </c>
+      <c r="J13">
+        <v>1638912</v>
+      </c>
+      <c r="K13" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="H14" t="s">
+        <v>93</v>
+      </c>
+      <c r="I14" t="s">
+        <v>91</v>
+      </c>
+      <c r="J14">
+        <v>0</v>
+      </c>
+      <c r="K14" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="H15" s="21" t="s">
+        <v>95</v>
+      </c>
+      <c r="I15" s="21" t="s">
+        <v>91</v>
+      </c>
+      <c r="J15" s="21">
+        <v>0</v>
+      </c>
+      <c r="K15" s="21" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="H16" t="s">
+        <v>97</v>
+      </c>
+      <c r="I16" t="s">
+        <v>43</v>
+      </c>
+      <c r="J16">
+        <v>5130</v>
+      </c>
+      <c r="K16" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="H17" s="20" t="s">
+        <v>99</v>
+      </c>
+      <c r="I17" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="J17" s="20">
+        <v>0</v>
+      </c>
+      <c r="K17" s="20" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="I18" t="s">
         <v>111</v>
       </c>
-      <c r="I11">
-        <v>0</v>
-      </c>
-      <c r="J11" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="G12" s="25" t="s">
-        <v>88</v>
-      </c>
-      <c r="H12" s="25" t="s">
-        <v>33</v>
-      </c>
-      <c r="I12" s="25">
-        <v>0</v>
-      </c>
-      <c r="J12" s="25" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="G13" t="s">
-        <v>91</v>
-      </c>
-      <c r="H13" t="s">
-        <v>92</v>
-      </c>
-      <c r="I13">
-        <v>1638912</v>
-      </c>
-      <c r="J13" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="G14" t="s">
-        <v>94</v>
-      </c>
-      <c r="H14" t="s">
-        <v>92</v>
-      </c>
-      <c r="I14">
-        <v>0</v>
-      </c>
-      <c r="J14" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="G15" s="25" t="s">
-        <v>96</v>
-      </c>
-      <c r="H15" s="25" t="s">
-        <v>92</v>
-      </c>
-      <c r="I15" s="25">
-        <v>0</v>
-      </c>
-      <c r="J15" s="25" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="G16" t="s">
-        <v>98</v>
-      </c>
-      <c r="H16" t="s">
-        <v>43</v>
-      </c>
-      <c r="I16">
-        <v>5130</v>
-      </c>
-      <c r="J16" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="17" spans="7:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="G17" s="24" t="s">
-        <v>100</v>
-      </c>
-      <c r="H17" s="24" t="s">
-        <v>43</v>
-      </c>
-      <c r="I17" s="24">
-        <v>0</v>
-      </c>
-      <c r="J17" s="24" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="18" spans="7:10" ht="17" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="H18" t="s">
-        <v>112</v>
-      </c>
-      <c r="I18">
+      <c r="J18">
         <v>1755466</v>
       </c>
     </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="C22" s="29" t="s">
+        <v>102</v>
+      </c>
+      <c r="D22" s="29"/>
+      <c r="E22" s="29"/>
+      <c r="F22" s="29"/>
+      <c r="G22" s="29"/>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="C23" s="26">
+        <v>32</v>
+      </c>
+      <c r="D23" s="26">
+        <v>64</v>
+      </c>
+      <c r="E23" s="26">
+        <v>128</v>
+      </c>
+      <c r="F23" s="26">
+        <v>256</v>
+      </c>
+      <c r="G23" s="26">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A24" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="B24" s="24">
+        <v>32</v>
+      </c>
+      <c r="C24" s="1">
+        <v>0.99170000000000003</v>
+      </c>
+      <c r="D24" s="1">
+        <v>0.99360000000000004</v>
+      </c>
+      <c r="E24" s="1">
+        <v>0.9929</v>
+      </c>
+      <c r="F24" s="1">
+        <v>0.99209999999999898</v>
+      </c>
+      <c r="G24" s="1">
+        <v>0.9919</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A25" s="31"/>
+      <c r="B25" s="24">
+        <v>128</v>
+      </c>
+      <c r="C25" s="1">
+        <v>0.99180000000000001</v>
+      </c>
+      <c r="D25" s="1">
+        <v>0.99109999999999898</v>
+      </c>
+      <c r="E25" s="1">
+        <v>0.99339999999999895</v>
+      </c>
+      <c r="F25" s="1">
+        <v>0.99350000000000005</v>
+      </c>
+      <c r="G25" s="1">
+        <v>0.99409999999999898</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A26" s="32"/>
+      <c r="B26" s="24">
+        <v>512</v>
+      </c>
+      <c r="C26" s="1">
+        <v>0.98780000000000001</v>
+      </c>
+      <c r="D26" s="1">
+        <v>0.99180000000000001</v>
+      </c>
+      <c r="E26" s="1">
+        <v>0.99229999999999896</v>
+      </c>
+      <c r="F26" s="1">
+        <v>0.99239999999999895</v>
+      </c>
+      <c r="G26" s="1">
+        <v>0.99390000000000001</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="4">
+    <mergeCell ref="A24:A26"/>
     <mergeCell ref="C3:E3"/>
     <mergeCell ref="A5:A9"/>
+    <mergeCell ref="C22:G22"/>
   </mergeCells>
-  <conditionalFormatting sqref="C5:E9">
+  <conditionalFormatting sqref="C5:F9">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C24:G26">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
@@ -2764,57 +3020,57 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>106</v>
-      </c>
-      <c r="I1" s="26" t="s">
-        <v>104</v>
+        <v>105</v>
+      </c>
+      <c r="I1" s="22" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C3" s="29" t="s">
-        <v>0</v>
-      </c>
-      <c r="D3" s="29"/>
-      <c r="E3" s="29"/>
-      <c r="I3" s="23" t="s">
+      <c r="C3" s="28" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" s="28"/>
+      <c r="E3" s="28"/>
+      <c r="I3" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="J3" s="23" t="s">
+      <c r="J3" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="K3" s="23" t="s">
+      <c r="K3" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="L3" s="23" t="s">
+      <c r="L3" s="19" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="17" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="C4" s="19">
+      <c r="C4" s="16">
         <v>32</v>
       </c>
-      <c r="D4" s="19">
+      <c r="D4" s="16">
         <v>128</v>
       </c>
-      <c r="E4" s="19">
+      <c r="E4" s="16">
         <v>512</v>
       </c>
       <c r="I4" t="s">
+        <v>64</v>
+      </c>
+      <c r="J4" t="s">
         <v>65</v>
-      </c>
-      <c r="J4" t="s">
-        <v>66</v>
       </c>
       <c r="K4">
         <v>1792</v>
       </c>
       <c r="L4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A5" s="30" t="s">
-        <v>103</v>
+      <c r="A5" s="29" t="s">
+        <v>102</v>
       </c>
       <c r="B5" s="2">
         <v>32</v>
@@ -2829,20 +3085,20 @@
         <v>0.55620000000000003</v>
       </c>
       <c r="I5" t="s">
+        <v>67</v>
+      </c>
+      <c r="J5" t="s">
+        <v>65</v>
+      </c>
+      <c r="K5">
+        <v>0</v>
+      </c>
+      <c r="L5" t="s">
         <v>68</v>
       </c>
-      <c r="J5" t="s">
-        <v>66</v>
-      </c>
-      <c r="K5">
-        <v>0</v>
-      </c>
-      <c r="L5" t="s">
-        <v>69</v>
-      </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A6" s="30"/>
+      <c r="A6" s="29"/>
       <c r="B6" s="2">
         <v>64</v>
       </c>
@@ -2855,21 +3111,21 @@
       <c r="E6" s="1">
         <v>0.56559999999999899</v>
       </c>
-      <c r="I6" s="25" t="s">
+      <c r="I6" s="21" t="s">
+        <v>69</v>
+      </c>
+      <c r="J6" s="21" t="s">
+        <v>65</v>
+      </c>
+      <c r="K6" s="21">
+        <v>0</v>
+      </c>
+      <c r="L6" s="21" t="s">
         <v>70</v>
       </c>
-      <c r="J6" s="25" t="s">
-        <v>66</v>
-      </c>
-      <c r="K6" s="25">
-        <v>0</v>
-      </c>
-      <c r="L6" s="25" t="s">
-        <v>71</v>
-      </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A7" s="30"/>
+      <c r="A7" s="29"/>
       <c r="B7" s="2">
         <v>128</v>
       </c>
@@ -2883,20 +3139,20 @@
         <v>0.60070000000000001</v>
       </c>
       <c r="I7" t="s">
+        <v>71</v>
+      </c>
+      <c r="J7" t="s">
         <v>72</v>
-      </c>
-      <c r="J7" t="s">
-        <v>73</v>
       </c>
       <c r="K7">
         <v>36928</v>
       </c>
       <c r="L7" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A8" s="30"/>
+      <c r="A8" s="29"/>
       <c r="B8" s="2">
         <v>256</v>
       </c>
@@ -2910,146 +3166,146 @@
         <v>0.61050000000000004</v>
       </c>
       <c r="I8" t="s">
+        <v>74</v>
+      </c>
+      <c r="J8" t="s">
+        <v>72</v>
+      </c>
+      <c r="K8">
+        <v>0</v>
+      </c>
+      <c r="L8" t="s">
         <v>75</v>
       </c>
-      <c r="J8" t="s">
-        <v>73</v>
-      </c>
-      <c r="K8">
-        <v>0</v>
-      </c>
-      <c r="L8" t="s">
-        <v>76</v>
-      </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A9" s="30"/>
+      <c r="A9" s="29"/>
       <c r="B9" s="2">
         <v>512</v>
       </c>
       <c r="C9" s="1">
         <v>0.71589999999999898</v>
       </c>
-      <c r="D9" s="27">
+      <c r="D9" s="23">
         <v>0.1</v>
       </c>
       <c r="E9" s="1">
         <v>0.63229999999999997</v>
       </c>
-      <c r="I9" s="25" t="s">
+      <c r="I9" s="21" t="s">
+        <v>76</v>
+      </c>
+      <c r="J9" s="21" t="s">
         <v>77</v>
       </c>
-      <c r="J9" s="25" t="s">
+      <c r="K9" s="21">
+        <v>0</v>
+      </c>
+      <c r="L9" s="21" t="s">
         <v>78</v>
-      </c>
-      <c r="K9" s="25">
-        <v>0</v>
-      </c>
-      <c r="L9" s="25" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="I10" t="s">
+        <v>79</v>
+      </c>
+      <c r="J10" t="s">
         <v>80</v>
-      </c>
-      <c r="J10" t="s">
-        <v>81</v>
       </c>
       <c r="K10">
         <v>73856</v>
       </c>
       <c r="L10" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="I11" t="s">
+        <v>82</v>
+      </c>
+      <c r="J11" t="s">
+        <v>80</v>
+      </c>
+      <c r="K11">
+        <v>0</v>
+      </c>
+      <c r="L11" t="s">
         <v>83</v>
-      </c>
-      <c r="J11" t="s">
-        <v>81</v>
-      </c>
-      <c r="K11">
-        <v>0</v>
-      </c>
-      <c r="L11" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="I12" t="s">
+        <v>84</v>
+      </c>
+      <c r="J12" t="s">
         <v>85</v>
       </c>
-      <c r="J12" t="s">
+      <c r="K12">
+        <v>0</v>
+      </c>
+      <c r="L12" t="s">
         <v>86</v>
       </c>
-      <c r="K12">
-        <v>0</v>
-      </c>
-      <c r="L12" t="s">
+    </row>
+    <row r="13" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I13" s="21" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="13" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="I13" s="25" t="s">
+      <c r="J13" s="21" t="s">
         <v>88</v>
       </c>
-      <c r="J13" s="25" t="s">
+      <c r="K13" s="21">
+        <v>0</v>
+      </c>
+      <c r="L13" s="21" t="s">
         <v>89</v>
-      </c>
-      <c r="K13" s="25">
-        <v>0</v>
-      </c>
-      <c r="L13" s="25" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="I14" t="s">
+        <v>90</v>
+      </c>
+      <c r="J14" t="s">
         <v>91</v>
-      </c>
-      <c r="J14" t="s">
-        <v>92</v>
       </c>
       <c r="K14">
         <v>2359808</v>
       </c>
       <c r="L14" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="I15" t="s">
+        <v>93</v>
+      </c>
+      <c r="J15" t="s">
+        <v>91</v>
+      </c>
+      <c r="K15">
+        <v>0</v>
+      </c>
+      <c r="L15" t="s">
         <v>94</v>
       </c>
-      <c r="J15" t="s">
-        <v>92</v>
-      </c>
-      <c r="K15">
-        <v>0</v>
-      </c>
-      <c r="L15" t="s">
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="I16" s="21" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="I16" s="25" t="s">
+      <c r="J16" s="21" t="s">
+        <v>91</v>
+      </c>
+      <c r="K16" s="21">
+        <v>0</v>
+      </c>
+      <c r="L16" s="21" t="s">
         <v>96</v>
-      </c>
-      <c r="J16" s="25" t="s">
-        <v>92</v>
-      </c>
-      <c r="K16" s="25">
-        <v>0</v>
-      </c>
-      <c r="L16" s="25" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="I17" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="J17" t="s">
         <v>43</v>
@@ -3058,62 +3314,62 @@
         <v>5130</v>
       </c>
       <c r="L17" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="I18" s="20" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="18" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="I18" s="24" t="s">
+      <c r="J18" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="K18" s="20">
+        <v>0</v>
+      </c>
+      <c r="L18" s="20" t="s">
         <v>100</v>
-      </c>
-      <c r="J18" s="24" t="s">
-        <v>43</v>
-      </c>
-      <c r="K18" s="24">
-        <v>0</v>
-      </c>
-      <c r="L18" s="24" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="19" spans="1:12" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="J19" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="K19">
         <v>2477514</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="C23" s="30" t="s">
-        <v>103</v>
-      </c>
-      <c r="D23" s="30"/>
-      <c r="E23" s="30"/>
-      <c r="F23" s="30"/>
-      <c r="G23" s="30"/>
+      <c r="C23" s="29" t="s">
+        <v>102</v>
+      </c>
+      <c r="D23" s="29"/>
+      <c r="E23" s="29"/>
+      <c r="F23" s="29"/>
+      <c r="G23" s="29"/>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="C24" s="19">
+      <c r="C24" s="16">
         <v>32</v>
       </c>
-      <c r="D24" s="19">
+      <c r="D24" s="16">
         <v>64</v>
       </c>
-      <c r="E24" s="19">
+      <c r="E24" s="16">
         <v>128</v>
       </c>
-      <c r="F24" s="19">
+      <c r="F24" s="16">
         <v>256</v>
       </c>
-      <c r="G24" s="19">
+      <c r="G24" s="16">
         <v>512</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A25" s="31" t="s">
-        <v>0</v>
-      </c>
-      <c r="B25" s="28">
+      <c r="A25" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="B25" s="24">
         <v>32</v>
       </c>
       <c r="C25" s="1">
@@ -3133,8 +3389,8 @@
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A26" s="32"/>
-      <c r="B26" s="28">
+      <c r="A26" s="31"/>
+      <c r="B26" s="24">
         <v>128</v>
       </c>
       <c r="C26" s="1">
@@ -3149,13 +3405,13 @@
       <c r="F26" s="1">
         <v>0.64970000000000006</v>
       </c>
-      <c r="G26" s="27">
+      <c r="G26" s="23">
         <v>0.1</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A27" s="33"/>
-      <c r="B27" s="28">
+      <c r="A27" s="32"/>
+      <c r="B27" s="24">
         <v>512</v>
       </c>
       <c r="C27" s="1">
@@ -3231,13 +3487,13 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="C4" s="29" t="s">
-        <v>0</v>
-      </c>
-      <c r="D4" s="29"/>
-      <c r="E4" s="29"/>
-      <c r="F4" s="29"/>
-      <c r="G4" s="29"/>
+      <c r="C4" s="28" t="s">
+        <v>0</v>
+      </c>
+      <c r="D4" s="28"/>
+      <c r="E4" s="28"/>
+      <c r="F4" s="28"/>
+      <c r="G4" s="28"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C5" s="2">
@@ -3257,7 +3513,7 @@
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6" s="30" t="s">
+      <c r="A6" s="29" t="s">
         <v>1</v>
       </c>
       <c r="B6" s="2">
@@ -3280,7 +3536,7 @@
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A7" s="30"/>
+      <c r="A7" s="29"/>
       <c r="B7" s="2">
         <v>8</v>
       </c>
@@ -3301,7 +3557,7 @@
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A8" s="30"/>
+      <c r="A8" s="29"/>
       <c r="B8" s="2">
         <v>16</v>
       </c>
@@ -3322,7 +3578,7 @@
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A9" s="30"/>
+      <c r="A9" s="29"/>
       <c r="B9" s="2">
         <v>32</v>
       </c>
@@ -3343,7 +3599,7 @@
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A10" s="30"/>
+      <c r="A10" s="29"/>
       <c r="B10" s="2">
         <v>64</v>
       </c>

</xml_diff>